<commit_message>
Site updated: 2025-01-19 23:15:26
</commit_message>
<xml_diff>
--- a/programs/periodic_table_4d.xlsx
+++ b/programs/periodic_table_4d.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Toccbai\do_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Toccbai\html5mijr\wxyroot\source\programs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F6C6E6-B898-4662-B3F7-E51732D69094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AFCB293-070D-45A1-B00C-55828D1A0175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="15" windowWidth="21585" windowHeight="12885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -550,9 +550,6 @@
     <t>Aa鈪</t>
   </si>
   <si>
-    <t>Ad鈄</t>
-  </si>
-  <si>
     <t>Cd镉</t>
   </si>
   <si>
@@ -15764,6 +15761,22 @@
         <charset val="134"/>
       </rPr>
       <t>4</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>Ad</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>钭</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -15772,7 +15785,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -15880,6 +15893,13 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Chemical4D"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
     </font>
@@ -16168,14 +16188,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -16183,11 +16197,11 @@
     <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -16195,13 +16209,19 @@
     <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -16464,8 +16484,8 @@
   </sheetPr>
   <dimension ref="A1:BM31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="Y1" sqref="Y1"/>
+    <sheetView tabSelected="1" topLeftCell="AC3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AR16" sqref="AR16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -16475,7 +16495,7 @@
   <sheetData>
     <row r="1" spans="1:65" ht="81" customHeight="1" x14ac:dyDescent="0.3">
       <c r="AA1" s="28" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="AB1" s="28"/>
       <c r="AC1" s="28"/>
@@ -16500,10 +16520,10 @@
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
       <c r="F2" s="27" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="G2" s="27" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
@@ -16558,10 +16578,10 @@
       <c r="BF2" s="19"/>
       <c r="BG2" s="19"/>
       <c r="BH2" s="27" t="s">
+        <v>355</v>
+      </c>
+      <c r="BI2" s="27" t="s">
         <v>356</v>
-      </c>
-      <c r="BI2" s="27" t="s">
-        <v>357</v>
       </c>
       <c r="BJ2" s="11"/>
       <c r="BK2" s="11"/>
@@ -16569,11 +16589,11 @@
       <c r="BM2" s="11"/>
     </row>
     <row r="3" spans="1:65" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="29"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="30">
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="33">
         <v>1</v>
       </c>
       <c r="F3" s="2">
@@ -16582,95 +16602,95 @@
       <c r="G3" s="2">
         <v>2</v>
       </c>
-      <c r="H3" s="36" t="s">
+      <c r="H3" s="34" t="s">
+        <v>357</v>
+      </c>
+      <c r="I3" s="30" t="s">
         <v>358</v>
       </c>
-      <c r="I3" s="32" t="s">
-        <v>359</v>
-      </c>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="29"/>
-      <c r="S3" s="29"/>
-      <c r="T3" s="29"/>
-      <c r="U3" s="29"/>
-      <c r="V3" s="29"/>
-      <c r="W3" s="29"/>
-      <c r="X3" s="29"/>
-      <c r="Y3" s="29"/>
-      <c r="Z3" s="29"/>
-      <c r="AA3" s="29"/>
-      <c r="AB3" s="29"/>
-      <c r="AC3" s="29"/>
-      <c r="AD3" s="29"/>
-      <c r="AE3" s="29"/>
-      <c r="AF3" s="29"/>
-      <c r="AG3" s="40" t="s">
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="32"/>
+      <c r="O3" s="32"/>
+      <c r="P3" s="32"/>
+      <c r="Q3" s="32"/>
+      <c r="R3" s="32"/>
+      <c r="S3" s="32"/>
+      <c r="T3" s="32"/>
+      <c r="U3" s="32"/>
+      <c r="V3" s="32"/>
+      <c r="W3" s="32"/>
+      <c r="X3" s="32"/>
+      <c r="Y3" s="32"/>
+      <c r="Z3" s="32"/>
+      <c r="AA3" s="32"/>
+      <c r="AB3" s="32"/>
+      <c r="AC3" s="32"/>
+      <c r="AD3" s="32"/>
+      <c r="AE3" s="32"/>
+      <c r="AF3" s="32"/>
+      <c r="AG3" s="39" t="s">
+        <v>431</v>
+      </c>
+      <c r="AH3" s="20"/>
+      <c r="AI3" s="29" t="s">
         <v>432</v>
       </c>
-      <c r="AH3" s="20"/>
-      <c r="AI3" s="39" t="s">
-        <v>433</v>
-      </c>
-      <c r="AJ3" s="39"/>
+      <c r="AJ3" s="29"/>
       <c r="AK3" s="21"/>
       <c r="AL3" s="22"/>
-      <c r="AM3" s="39" t="s">
-        <v>434</v>
+      <c r="AM3" s="29" t="s">
+        <v>433</v>
       </c>
       <c r="AN3" s="21"/>
       <c r="AO3" s="21"/>
       <c r="AP3" s="21"/>
       <c r="AQ3" s="21"/>
-      <c r="AR3" s="29"/>
-      <c r="AS3" s="29"/>
-      <c r="AT3" s="32" t="s">
+      <c r="AR3" s="32"/>
+      <c r="AS3" s="32"/>
+      <c r="AT3" s="30" t="s">
+        <v>359</v>
+      </c>
+      <c r="AU3" s="30" t="s">
         <v>360</v>
       </c>
-      <c r="AU3" s="32" t="s">
+      <c r="AV3" s="30" t="s">
         <v>361</v>
       </c>
-      <c r="AV3" s="32" t="s">
+      <c r="AW3" s="30" t="s">
         <v>362</v>
       </c>
-      <c r="AW3" s="32" t="s">
+      <c r="AX3" s="30" t="s">
         <v>363</v>
       </c>
-      <c r="AX3" s="32" t="s">
+      <c r="AY3" s="30" t="s">
         <v>364</v>
       </c>
-      <c r="AY3" s="32" t="s">
+      <c r="AZ3" s="30" t="s">
         <v>365</v>
       </c>
-      <c r="AZ3" s="32" t="s">
+      <c r="BA3" s="30" t="s">
         <v>366</v>
       </c>
-      <c r="BA3" s="32" t="s">
+      <c r="BB3" s="30" t="s">
         <v>367</v>
       </c>
-      <c r="BB3" s="32" t="s">
+      <c r="BC3" s="30" t="s">
         <v>368</v>
       </c>
-      <c r="BC3" s="32" t="s">
+      <c r="BD3" s="30" t="s">
         <v>369</v>
       </c>
-      <c r="BD3" s="32" t="s">
+      <c r="BE3" s="30" t="s">
         <v>370</v>
       </c>
-      <c r="BE3" s="32" t="s">
+      <c r="BF3" s="30" t="s">
         <v>371</v>
       </c>
-      <c r="BF3" s="32" t="s">
+      <c r="BG3" s="37" t="s">
         <v>372</v>
-      </c>
-      <c r="BG3" s="34" t="s">
-        <v>373</v>
       </c>
       <c r="BH3" s="2">
         <v>3</v>
@@ -16678,169 +16698,169 @@
       <c r="BI3" s="3">
         <v>4</v>
       </c>
-      <c r="BJ3" s="31"/>
-      <c r="BK3" s="29"/>
-      <c r="BL3" s="29"/>
-      <c r="BM3" s="29"/>
+      <c r="BJ3" s="36"/>
+      <c r="BK3" s="32"/>
+      <c r="BL3" s="32"/>
+      <c r="BM3" s="32"/>
     </row>
     <row r="4" spans="1:65" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="29"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="30"/>
+      <c r="A4" s="32"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="33"/>
       <c r="F4" s="7" t="s">
         <v>0</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="36"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
-      <c r="O4" s="29"/>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="29"/>
-      <c r="R4" s="29"/>
-      <c r="S4" s="29"/>
-      <c r="T4" s="29"/>
-      <c r="U4" s="29"/>
-      <c r="V4" s="29"/>
-      <c r="W4" s="29"/>
-      <c r="X4" s="29"/>
-      <c r="Y4" s="29"/>
-      <c r="Z4" s="29"/>
-      <c r="AA4" s="29"/>
-      <c r="AB4" s="29"/>
-      <c r="AC4" s="29"/>
-      <c r="AD4" s="29"/>
-      <c r="AE4" s="29"/>
-      <c r="AF4" s="29"/>
-      <c r="AG4" s="40"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="32"/>
+      <c r="M4" s="32"/>
+      <c r="N4" s="32"/>
+      <c r="O4" s="32"/>
+      <c r="P4" s="32"/>
+      <c r="Q4" s="32"/>
+      <c r="R4" s="32"/>
+      <c r="S4" s="32"/>
+      <c r="T4" s="32"/>
+      <c r="U4" s="32"/>
+      <c r="V4" s="32"/>
+      <c r="W4" s="32"/>
+      <c r="X4" s="32"/>
+      <c r="Y4" s="32"/>
+      <c r="Z4" s="32"/>
+      <c r="AA4" s="32"/>
+      <c r="AB4" s="32"/>
+      <c r="AC4" s="32"/>
+      <c r="AD4" s="32"/>
+      <c r="AE4" s="32"/>
+      <c r="AF4" s="32"/>
+      <c r="AG4" s="39"/>
       <c r="AH4" s="23"/>
-      <c r="AI4" s="39"/>
-      <c r="AJ4" s="39"/>
+      <c r="AI4" s="29"/>
+      <c r="AJ4" s="29"/>
       <c r="AK4" s="24"/>
       <c r="AL4" s="22"/>
-      <c r="AM4" s="39"/>
+      <c r="AM4" s="29"/>
       <c r="AN4" s="25"/>
       <c r="AO4" s="21"/>
       <c r="AP4" s="22" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="AQ4" s="26"/>
-      <c r="AR4" s="29"/>
-      <c r="AS4" s="29"/>
-      <c r="AT4" s="32"/>
-      <c r="AU4" s="32"/>
-      <c r="AV4" s="32"/>
-      <c r="AW4" s="32"/>
-      <c r="AX4" s="32"/>
-      <c r="AY4" s="32"/>
-      <c r="AZ4" s="32"/>
-      <c r="BA4" s="32"/>
-      <c r="BB4" s="32"/>
-      <c r="BC4" s="32"/>
-      <c r="BD4" s="32"/>
-      <c r="BE4" s="32"/>
-      <c r="BF4" s="32"/>
-      <c r="BG4" s="34"/>
+      <c r="AR4" s="32"/>
+      <c r="AS4" s="32"/>
+      <c r="AT4" s="30"/>
+      <c r="AU4" s="30"/>
+      <c r="AV4" s="30"/>
+      <c r="AW4" s="30"/>
+      <c r="AX4" s="30"/>
+      <c r="AY4" s="30"/>
+      <c r="AZ4" s="30"/>
+      <c r="BA4" s="30"/>
+      <c r="BB4" s="30"/>
+      <c r="BC4" s="30"/>
+      <c r="BD4" s="30"/>
+      <c r="BE4" s="30"/>
+      <c r="BF4" s="30"/>
+      <c r="BG4" s="37"/>
       <c r="BH4" s="7" t="s">
         <v>2</v>
       </c>
       <c r="BI4" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="BJ4" s="31"/>
-      <c r="BK4" s="29"/>
-      <c r="BL4" s="29"/>
-      <c r="BM4" s="29"/>
+      <c r="BJ4" s="36"/>
+      <c r="BK4" s="32"/>
+      <c r="BL4" s="32"/>
+      <c r="BM4" s="32"/>
     </row>
     <row r="5" spans="1:65" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="29"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="30"/>
+      <c r="A5" s="32"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="33"/>
       <c r="F5" s="12" t="s">
+        <v>456</v>
+      </c>
+      <c r="G5" s="12" t="s">
         <v>457</v>
       </c>
-      <c r="G5" s="12" t="s">
-        <v>458</v>
-      </c>
-      <c r="H5" s="37"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
-      <c r="O5" s="29"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="29"/>
-      <c r="R5" s="29"/>
-      <c r="S5" s="29"/>
-      <c r="T5" s="29"/>
-      <c r="U5" s="29"/>
-      <c r="V5" s="29"/>
-      <c r="W5" s="29"/>
-      <c r="X5" s="29"/>
-      <c r="Y5" s="29"/>
-      <c r="Z5" s="29"/>
-      <c r="AA5" s="29"/>
-      <c r="AB5" s="29"/>
-      <c r="AC5" s="29"/>
-      <c r="AD5" s="29"/>
-      <c r="AE5" s="29"/>
-      <c r="AF5" s="29"/>
-      <c r="AG5" s="40"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="32"/>
+      <c r="N5" s="32"/>
+      <c r="O5" s="32"/>
+      <c r="P5" s="32"/>
+      <c r="Q5" s="32"/>
+      <c r="R5" s="32"/>
+      <c r="S5" s="32"/>
+      <c r="T5" s="32"/>
+      <c r="U5" s="32"/>
+      <c r="V5" s="32"/>
+      <c r="W5" s="32"/>
+      <c r="X5" s="32"/>
+      <c r="Y5" s="32"/>
+      <c r="Z5" s="32"/>
+      <c r="AA5" s="32"/>
+      <c r="AB5" s="32"/>
+      <c r="AC5" s="32"/>
+      <c r="AD5" s="32"/>
+      <c r="AE5" s="32"/>
+      <c r="AF5" s="32"/>
+      <c r="AG5" s="39"/>
       <c r="AH5" s="20"/>
-      <c r="AI5" s="39"/>
-      <c r="AJ5" s="39"/>
+      <c r="AI5" s="29"/>
+      <c r="AJ5" s="29"/>
       <c r="AK5" s="20"/>
       <c r="AL5" s="22"/>
-      <c r="AM5" s="39"/>
+      <c r="AM5" s="29"/>
       <c r="AN5" s="21"/>
       <c r="AO5" s="21"/>
       <c r="AP5" s="21"/>
       <c r="AQ5" s="21"/>
-      <c r="AR5" s="29"/>
-      <c r="AS5" s="29"/>
-      <c r="AT5" s="33"/>
-      <c r="AU5" s="33"/>
-      <c r="AV5" s="33"/>
-      <c r="AW5" s="33"/>
-      <c r="AX5" s="33"/>
-      <c r="AY5" s="33"/>
-      <c r="AZ5" s="33"/>
-      <c r="BA5" s="33"/>
-      <c r="BB5" s="33"/>
-      <c r="BC5" s="33"/>
-      <c r="BD5" s="33"/>
-      <c r="BE5" s="33"/>
-      <c r="BF5" s="33"/>
-      <c r="BG5" s="35"/>
+      <c r="AR5" s="32"/>
+      <c r="AS5" s="32"/>
+      <c r="AT5" s="31"/>
+      <c r="AU5" s="31"/>
+      <c r="AV5" s="31"/>
+      <c r="AW5" s="31"/>
+      <c r="AX5" s="31"/>
+      <c r="AY5" s="31"/>
+      <c r="AZ5" s="31"/>
+      <c r="BA5" s="31"/>
+      <c r="BB5" s="31"/>
+      <c r="BC5" s="31"/>
+      <c r="BD5" s="31"/>
+      <c r="BE5" s="31"/>
+      <c r="BF5" s="31"/>
+      <c r="BG5" s="38"/>
       <c r="BH5" s="12" t="s">
+        <v>458</v>
+      </c>
+      <c r="BI5" s="18" t="s">
         <v>459</v>
       </c>
-      <c r="BI5" s="18" t="s">
-        <v>460</v>
-      </c>
-      <c r="BJ5" s="31"/>
-      <c r="BK5" s="29"/>
-      <c r="BL5" s="29"/>
-      <c r="BM5" s="29"/>
+      <c r="BJ5" s="36"/>
+      <c r="BK5" s="32"/>
+      <c r="BL5" s="32"/>
+      <c r="BM5" s="32"/>
     </row>
     <row r="6" spans="1:65" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="29"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="30">
+      <c r="A6" s="32"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="33">
         <v>2</v>
       </c>
       <c r="F6" s="4">
@@ -16855,42 +16875,42 @@
       <c r="I6" s="4">
         <v>8</v>
       </c>
-      <c r="J6" s="31"/>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
-      <c r="O6" s="29"/>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="29"/>
-      <c r="R6" s="29"/>
-      <c r="S6" s="29"/>
-      <c r="T6" s="29"/>
-      <c r="U6" s="29"/>
-      <c r="V6" s="29"/>
-      <c r="W6" s="29"/>
-      <c r="X6" s="29"/>
-      <c r="Y6" s="29"/>
-      <c r="Z6" s="29"/>
-      <c r="AA6" s="29"/>
-      <c r="AB6" s="29"/>
-      <c r="AC6" s="29"/>
-      <c r="AD6" s="29"/>
-      <c r="AE6" s="29"/>
-      <c r="AF6" s="29"/>
-      <c r="AG6" s="29"/>
-      <c r="AH6" s="29"/>
-      <c r="AI6" s="29"/>
-      <c r="AJ6" s="29"/>
-      <c r="AK6" s="29"/>
-      <c r="AL6" s="29"/>
-      <c r="AM6" s="29"/>
-      <c r="AN6" s="29"/>
-      <c r="AO6" s="29"/>
-      <c r="AP6" s="29"/>
-      <c r="AQ6" s="29"/>
-      <c r="AR6" s="29"/>
-      <c r="AS6" s="38"/>
+      <c r="J6" s="36"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="32"/>
+      <c r="N6" s="32"/>
+      <c r="O6" s="32"/>
+      <c r="P6" s="32"/>
+      <c r="Q6" s="32"/>
+      <c r="R6" s="32"/>
+      <c r="S6" s="32"/>
+      <c r="T6" s="32"/>
+      <c r="U6" s="32"/>
+      <c r="V6" s="32"/>
+      <c r="W6" s="32"/>
+      <c r="X6" s="32"/>
+      <c r="Y6" s="32"/>
+      <c r="Z6" s="32"/>
+      <c r="AA6" s="32"/>
+      <c r="AB6" s="32"/>
+      <c r="AC6" s="32"/>
+      <c r="AD6" s="32"/>
+      <c r="AE6" s="32"/>
+      <c r="AF6" s="32"/>
+      <c r="AG6" s="32"/>
+      <c r="AH6" s="32"/>
+      <c r="AI6" s="32"/>
+      <c r="AJ6" s="32"/>
+      <c r="AK6" s="32"/>
+      <c r="AL6" s="32"/>
+      <c r="AM6" s="32"/>
+      <c r="AN6" s="32"/>
+      <c r="AO6" s="32"/>
+      <c r="AP6" s="32"/>
+      <c r="AQ6" s="32"/>
+      <c r="AR6" s="32"/>
+      <c r="AS6" s="40"/>
       <c r="AT6" s="2">
         <v>9</v>
       </c>
@@ -16939,17 +16959,17 @@
       <c r="BI6" s="3">
         <v>24</v>
       </c>
-      <c r="BJ6" s="31"/>
-      <c r="BK6" s="29"/>
-      <c r="BL6" s="29"/>
-      <c r="BM6" s="29"/>
+      <c r="BJ6" s="36"/>
+      <c r="BK6" s="32"/>
+      <c r="BL6" s="32"/>
+      <c r="BM6" s="32"/>
     </row>
     <row r="7" spans="1:65" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="29"/>
-      <c r="B7" s="29"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="30"/>
+      <c r="A7" s="32"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="33"/>
       <c r="F7" s="8" t="s">
         <v>4</v>
       </c>
@@ -16962,42 +16982,42 @@
       <c r="I7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="31"/>
-      <c r="K7" s="29"/>
-      <c r="L7" s="29"/>
-      <c r="M7" s="29"/>
-      <c r="N7" s="29"/>
-      <c r="O7" s="29"/>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="29"/>
-      <c r="R7" s="29"/>
-      <c r="S7" s="29"/>
-      <c r="T7" s="29"/>
-      <c r="U7" s="29"/>
-      <c r="V7" s="29"/>
-      <c r="W7" s="29"/>
-      <c r="X7" s="29"/>
-      <c r="Y7" s="29"/>
-      <c r="Z7" s="29"/>
-      <c r="AA7" s="29"/>
-      <c r="AB7" s="29"/>
-      <c r="AC7" s="29"/>
-      <c r="AD7" s="29"/>
-      <c r="AE7" s="29"/>
-      <c r="AF7" s="29"/>
-      <c r="AG7" s="29"/>
-      <c r="AH7" s="29"/>
-      <c r="AI7" s="29"/>
-      <c r="AJ7" s="29"/>
-      <c r="AK7" s="29"/>
-      <c r="AL7" s="29"/>
-      <c r="AM7" s="29"/>
-      <c r="AN7" s="29"/>
-      <c r="AO7" s="29"/>
-      <c r="AP7" s="29"/>
-      <c r="AQ7" s="29"/>
-      <c r="AR7" s="29"/>
-      <c r="AS7" s="38"/>
+      <c r="J7" s="36"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="32"/>
+      <c r="N7" s="32"/>
+      <c r="O7" s="32"/>
+      <c r="P7" s="32"/>
+      <c r="Q7" s="32"/>
+      <c r="R7" s="32"/>
+      <c r="S7" s="32"/>
+      <c r="T7" s="32"/>
+      <c r="U7" s="32"/>
+      <c r="V7" s="32"/>
+      <c r="W7" s="32"/>
+      <c r="X7" s="32"/>
+      <c r="Y7" s="32"/>
+      <c r="Z7" s="32"/>
+      <c r="AA7" s="32"/>
+      <c r="AB7" s="32"/>
+      <c r="AC7" s="32"/>
+      <c r="AD7" s="32"/>
+      <c r="AE7" s="32"/>
+      <c r="AF7" s="32"/>
+      <c r="AG7" s="32"/>
+      <c r="AH7" s="32"/>
+      <c r="AI7" s="32"/>
+      <c r="AJ7" s="32"/>
+      <c r="AK7" s="32"/>
+      <c r="AL7" s="32"/>
+      <c r="AM7" s="32"/>
+      <c r="AN7" s="32"/>
+      <c r="AO7" s="32"/>
+      <c r="AP7" s="32"/>
+      <c r="AQ7" s="32"/>
+      <c r="AR7" s="32"/>
+      <c r="AS7" s="40"/>
       <c r="AT7" s="7" t="s">
         <v>8</v>
       </c>
@@ -17029,7 +17049,7 @@
         <v>17</v>
       </c>
       <c r="BD7" s="7" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="BE7" s="7" t="s">
         <v>18</v>
@@ -17046,124 +17066,124 @@
       <c r="BI7" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="BJ7" s="31"/>
-      <c r="BK7" s="29"/>
-      <c r="BL7" s="29"/>
-      <c r="BM7" s="29"/>
+      <c r="BJ7" s="36"/>
+      <c r="BK7" s="32"/>
+      <c r="BL7" s="32"/>
+      <c r="BM7" s="32"/>
     </row>
     <row r="8" spans="1:65" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="29"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="30"/>
+      <c r="A8" s="32"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="33"/>
       <c r="F8" s="13" t="s">
+        <v>460</v>
+      </c>
+      <c r="G8" s="13" t="s">
         <v>461</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="H8" s="13" t="s">
         <v>462</v>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="I8" s="13" t="s">
         <v>463</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="J8" s="36"/>
+      <c r="K8" s="32"/>
+      <c r="L8" s="32"/>
+      <c r="M8" s="32"/>
+      <c r="N8" s="32"/>
+      <c r="O8" s="32"/>
+      <c r="P8" s="32"/>
+      <c r="Q8" s="32"/>
+      <c r="R8" s="32"/>
+      <c r="S8" s="32"/>
+      <c r="T8" s="32"/>
+      <c r="U8" s="32"/>
+      <c r="V8" s="32"/>
+      <c r="W8" s="32"/>
+      <c r="X8" s="32"/>
+      <c r="Y8" s="32"/>
+      <c r="Z8" s="32"/>
+      <c r="AA8" s="32"/>
+      <c r="AB8" s="32"/>
+      <c r="AC8" s="32"/>
+      <c r="AD8" s="32"/>
+      <c r="AE8" s="32"/>
+      <c r="AF8" s="32"/>
+      <c r="AG8" s="32"/>
+      <c r="AH8" s="32"/>
+      <c r="AI8" s="32"/>
+      <c r="AJ8" s="32"/>
+      <c r="AK8" s="32"/>
+      <c r="AL8" s="32"/>
+      <c r="AM8" s="32"/>
+      <c r="AN8" s="32"/>
+      <c r="AO8" s="32"/>
+      <c r="AP8" s="32"/>
+      <c r="AQ8" s="32"/>
+      <c r="AR8" s="32"/>
+      <c r="AS8" s="40"/>
+      <c r="AT8" s="12" t="s">
         <v>464</v>
       </c>
-      <c r="J8" s="31"/>
-      <c r="K8" s="29"/>
-      <c r="L8" s="29"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="29"/>
-      <c r="O8" s="29"/>
-      <c r="P8" s="29"/>
-      <c r="Q8" s="29"/>
-      <c r="R8" s="29"/>
-      <c r="S8" s="29"/>
-      <c r="T8" s="29"/>
-      <c r="U8" s="29"/>
-      <c r="V8" s="29"/>
-      <c r="W8" s="29"/>
-      <c r="X8" s="29"/>
-      <c r="Y8" s="29"/>
-      <c r="Z8" s="29"/>
-      <c r="AA8" s="29"/>
-      <c r="AB8" s="29"/>
-      <c r="AC8" s="29"/>
-      <c r="AD8" s="29"/>
-      <c r="AE8" s="29"/>
-      <c r="AF8" s="29"/>
-      <c r="AG8" s="29"/>
-      <c r="AH8" s="29"/>
-      <c r="AI8" s="29"/>
-      <c r="AJ8" s="29"/>
-      <c r="AK8" s="29"/>
-      <c r="AL8" s="29"/>
-      <c r="AM8" s="29"/>
-      <c r="AN8" s="29"/>
-      <c r="AO8" s="29"/>
-      <c r="AP8" s="29"/>
-      <c r="AQ8" s="29"/>
-      <c r="AR8" s="29"/>
-      <c r="AS8" s="38"/>
-      <c r="AT8" s="12" t="s">
+      <c r="AU8" s="12" t="s">
         <v>465</v>
       </c>
-      <c r="AU8" s="12" t="s">
+      <c r="AV8" s="12" t="s">
         <v>466</v>
       </c>
-      <c r="AV8" s="12" t="s">
+      <c r="AW8" s="12" t="s">
         <v>467</v>
       </c>
-      <c r="AW8" s="12" t="s">
+      <c r="AX8" s="12" t="s">
         <v>468</v>
       </c>
-      <c r="AX8" s="12" t="s">
+      <c r="AY8" s="12" t="s">
         <v>469</v>
       </c>
-      <c r="AY8" s="12" t="s">
+      <c r="AZ8" s="12" t="s">
         <v>470</v>
       </c>
-      <c r="AZ8" s="12" t="s">
+      <c r="BA8" s="12" t="s">
         <v>471</v>
       </c>
-      <c r="BA8" s="12" t="s">
+      <c r="BB8" s="12" t="s">
         <v>472</v>
       </c>
-      <c r="BB8" s="12" t="s">
+      <c r="BC8" s="12" t="s">
         <v>473</v>
       </c>
-      <c r="BC8" s="12" t="s">
+      <c r="BD8" s="12" t="s">
         <v>474</v>
       </c>
-      <c r="BD8" s="12" t="s">
+      <c r="BE8" s="12" t="s">
         <v>475</v>
       </c>
-      <c r="BE8" s="12" t="s">
+      <c r="BF8" s="12" t="s">
         <v>476</v>
       </c>
-      <c r="BF8" s="12" t="s">
+      <c r="BG8" s="12" t="s">
         <v>477</v>
       </c>
-      <c r="BG8" s="12" t="s">
+      <c r="BH8" s="12" t="s">
         <v>478</v>
       </c>
-      <c r="BH8" s="12" t="s">
+      <c r="BI8" s="18" t="s">
         <v>479</v>
       </c>
-      <c r="BI8" s="18" t="s">
-        <v>480</v>
-      </c>
-      <c r="BJ8" s="31"/>
-      <c r="BK8" s="29"/>
-      <c r="BL8" s="29"/>
-      <c r="BM8" s="29"/>
+      <c r="BJ8" s="36"/>
+      <c r="BK8" s="32"/>
+      <c r="BL8" s="32"/>
+      <c r="BM8" s="32"/>
     </row>
     <row r="9" spans="1:65" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="29"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="30">
+      <c r="A9" s="32"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="33">
         <v>3</v>
       </c>
       <c r="F9" s="4">
@@ -17178,113 +17198,113 @@
       <c r="I9" s="4">
         <v>28</v>
       </c>
-      <c r="J9" s="36" t="s">
+      <c r="J9" s="34" t="s">
+        <v>374</v>
+      </c>
+      <c r="K9" s="30" t="s">
         <v>375</v>
       </c>
-      <c r="K9" s="32" t="s">
+      <c r="L9" s="30" t="s">
         <v>376</v>
       </c>
-      <c r="L9" s="32" t="s">
+      <c r="M9" s="30" t="s">
         <v>377</v>
       </c>
-      <c r="M9" s="32" t="s">
+      <c r="N9" s="30" t="s">
         <v>378</v>
       </c>
-      <c r="N9" s="32" t="s">
+      <c r="O9" s="30" t="s">
         <v>379</v>
       </c>
-      <c r="O9" s="32" t="s">
+      <c r="P9" s="30" t="s">
         <v>380</v>
       </c>
-      <c r="P9" s="32" t="s">
+      <c r="Q9" s="30" t="s">
         <v>381</v>
       </c>
-      <c r="Q9" s="32" t="s">
+      <c r="R9" s="30" t="s">
         <v>382</v>
       </c>
-      <c r="R9" s="32" t="s">
+      <c r="S9" s="30" t="s">
         <v>383</v>
       </c>
-      <c r="S9" s="32" t="s">
+      <c r="T9" s="30" t="s">
         <v>384</v>
       </c>
-      <c r="T9" s="32" t="s">
+      <c r="U9" s="30" t="s">
         <v>385</v>
       </c>
-      <c r="U9" s="32" t="s">
+      <c r="V9" s="30" t="s">
         <v>386</v>
       </c>
-      <c r="V9" s="32" t="s">
+      <c r="W9" s="30" t="s">
         <v>387</v>
       </c>
-      <c r="W9" s="32" t="s">
+      <c r="X9" s="30" t="s">
         <v>388</v>
       </c>
-      <c r="X9" s="32" t="s">
+      <c r="Y9" s="30" t="s">
         <v>389</v>
       </c>
-      <c r="Y9" s="32" t="s">
+      <c r="Z9" s="30" t="s">
         <v>390</v>
       </c>
-      <c r="Z9" s="32" t="s">
+      <c r="AA9" s="30" t="s">
         <v>391</v>
       </c>
-      <c r="AA9" s="32" t="s">
+      <c r="AB9" s="30" t="s">
         <v>392</v>
       </c>
-      <c r="AB9" s="32" t="s">
+      <c r="AC9" s="30" t="s">
         <v>393</v>
       </c>
-      <c r="AC9" s="32" t="s">
+      <c r="AD9" s="30" t="s">
         <v>394</v>
       </c>
-      <c r="AD9" s="32" t="s">
+      <c r="AE9" s="30" t="s">
         <v>395</v>
       </c>
-      <c r="AE9" s="32" t="s">
+      <c r="AF9" s="30" t="s">
         <v>396</v>
       </c>
-      <c r="AF9" s="32" t="s">
+      <c r="AG9" s="30" t="s">
         <v>397</v>
       </c>
-      <c r="AG9" s="32" t="s">
+      <c r="AH9" s="30" t="s">
         <v>398</v>
       </c>
-      <c r="AH9" s="32" t="s">
+      <c r="AI9" s="30" t="s">
         <v>399</v>
       </c>
-      <c r="AI9" s="32" t="s">
+      <c r="AJ9" s="30" t="s">
         <v>400</v>
       </c>
-      <c r="AJ9" s="32" t="s">
+      <c r="AK9" s="30" t="s">
         <v>401</v>
       </c>
-      <c r="AK9" s="32" t="s">
+      <c r="AL9" s="30" t="s">
         <v>402</v>
       </c>
-      <c r="AL9" s="32" t="s">
+      <c r="AM9" s="30" t="s">
         <v>403</v>
       </c>
-      <c r="AM9" s="32" t="s">
+      <c r="AN9" s="30" t="s">
         <v>404</v>
       </c>
-      <c r="AN9" s="32" t="s">
+      <c r="AO9" s="30" t="s">
         <v>405</v>
       </c>
-      <c r="AO9" s="32" t="s">
+      <c r="AP9" s="30" t="s">
         <v>406</v>
       </c>
-      <c r="AP9" s="32" t="s">
+      <c r="AQ9" s="30" t="s">
         <v>407</v>
       </c>
-      <c r="AQ9" s="32" t="s">
+      <c r="AR9" s="30" t="s">
         <v>408</v>
       </c>
-      <c r="AR9" s="32" t="s">
+      <c r="AS9" s="37" t="s">
         <v>409</v>
-      </c>
-      <c r="AS9" s="34" t="s">
-        <v>410</v>
       </c>
       <c r="AT9" s="4">
         <v>29</v>
@@ -17334,17 +17354,17 @@
       <c r="BI9" s="3">
         <v>44</v>
       </c>
-      <c r="BJ9" s="31"/>
-      <c r="BK9" s="29"/>
-      <c r="BL9" s="29"/>
-      <c r="BM9" s="29"/>
+      <c r="BJ9" s="36"/>
+      <c r="BK9" s="32"/>
+      <c r="BL9" s="32"/>
+      <c r="BM9" s="32"/>
     </row>
     <row r="10" spans="1:65" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="29"/>
-      <c r="B10" s="29"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="30"/>
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="33"/>
       <c r="F10" s="8" t="s">
         <v>23</v>
       </c>
@@ -17352,47 +17372,47 @@
         <v>24</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="I10" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="J10" s="36"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="32"/>
-      <c r="M10" s="32"/>
-      <c r="N10" s="32"/>
-      <c r="O10" s="32"/>
-      <c r="P10" s="32"/>
-      <c r="Q10" s="32"/>
-      <c r="R10" s="32"/>
-      <c r="S10" s="32"/>
-      <c r="T10" s="32"/>
-      <c r="U10" s="32"/>
-      <c r="V10" s="32"/>
-      <c r="W10" s="32"/>
-      <c r="X10" s="32"/>
-      <c r="Y10" s="32"/>
-      <c r="Z10" s="32"/>
-      <c r="AA10" s="32"/>
-      <c r="AB10" s="32"/>
-      <c r="AC10" s="32"/>
-      <c r="AD10" s="32"/>
-      <c r="AE10" s="32"/>
-      <c r="AF10" s="32"/>
-      <c r="AG10" s="32"/>
-      <c r="AH10" s="32"/>
-      <c r="AI10" s="32"/>
-      <c r="AJ10" s="32"/>
-      <c r="AK10" s="32"/>
-      <c r="AL10" s="32"/>
-      <c r="AM10" s="32"/>
-      <c r="AN10" s="32"/>
-      <c r="AO10" s="32"/>
-      <c r="AP10" s="32"/>
-      <c r="AQ10" s="32"/>
-      <c r="AR10" s="32"/>
-      <c r="AS10" s="34"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="30"/>
+      <c r="O10" s="30"/>
+      <c r="P10" s="30"/>
+      <c r="Q10" s="30"/>
+      <c r="R10" s="30"/>
+      <c r="S10" s="30"/>
+      <c r="T10" s="30"/>
+      <c r="U10" s="30"/>
+      <c r="V10" s="30"/>
+      <c r="W10" s="30"/>
+      <c r="X10" s="30"/>
+      <c r="Y10" s="30"/>
+      <c r="Z10" s="30"/>
+      <c r="AA10" s="30"/>
+      <c r="AB10" s="30"/>
+      <c r="AC10" s="30"/>
+      <c r="AD10" s="30"/>
+      <c r="AE10" s="30"/>
+      <c r="AF10" s="30"/>
+      <c r="AG10" s="30"/>
+      <c r="AH10" s="30"/>
+      <c r="AI10" s="30"/>
+      <c r="AJ10" s="30"/>
+      <c r="AK10" s="30"/>
+      <c r="AL10" s="30"/>
+      <c r="AM10" s="30"/>
+      <c r="AN10" s="30"/>
+      <c r="AO10" s="30"/>
+      <c r="AP10" s="30"/>
+      <c r="AQ10" s="30"/>
+      <c r="AR10" s="30"/>
+      <c r="AS10" s="37"/>
       <c r="AT10" s="8" t="s">
         <v>26</v>
       </c>
@@ -17441,124 +17461,124 @@
       <c r="BI10" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="BJ10" s="31"/>
-      <c r="BK10" s="29"/>
-      <c r="BL10" s="29"/>
-      <c r="BM10" s="29"/>
+      <c r="BJ10" s="36"/>
+      <c r="BK10" s="32"/>
+      <c r="BL10" s="32"/>
+      <c r="BM10" s="32"/>
     </row>
     <row r="11" spans="1:65" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="29"/>
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="30"/>
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="33"/>
       <c r="F11" s="13" t="s">
+        <v>480</v>
+      </c>
+      <c r="G11" s="13" t="s">
         <v>481</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="H11" s="13" t="s">
         <v>482</v>
       </c>
-      <c r="H11" s="13" t="s">
+      <c r="I11" s="13" t="s">
         <v>483</v>
       </c>
-      <c r="I11" s="13" t="s">
+      <c r="J11" s="35"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="31"/>
+      <c r="O11" s="31"/>
+      <c r="P11" s="31"/>
+      <c r="Q11" s="31"/>
+      <c r="R11" s="31"/>
+      <c r="S11" s="31"/>
+      <c r="T11" s="31"/>
+      <c r="U11" s="31"/>
+      <c r="V11" s="31"/>
+      <c r="W11" s="31"/>
+      <c r="X11" s="31"/>
+      <c r="Y11" s="31"/>
+      <c r="Z11" s="31"/>
+      <c r="AA11" s="31"/>
+      <c r="AB11" s="31"/>
+      <c r="AC11" s="31"/>
+      <c r="AD11" s="31"/>
+      <c r="AE11" s="31"/>
+      <c r="AF11" s="31"/>
+      <c r="AG11" s="31"/>
+      <c r="AH11" s="31"/>
+      <c r="AI11" s="31"/>
+      <c r="AJ11" s="31"/>
+      <c r="AK11" s="31"/>
+      <c r="AL11" s="31"/>
+      <c r="AM11" s="31"/>
+      <c r="AN11" s="31"/>
+      <c r="AO11" s="31"/>
+      <c r="AP11" s="31"/>
+      <c r="AQ11" s="31"/>
+      <c r="AR11" s="31"/>
+      <c r="AS11" s="38"/>
+      <c r="AT11" s="13" t="s">
         <v>484</v>
       </c>
-      <c r="J11" s="37"/>
-      <c r="K11" s="33"/>
-      <c r="L11" s="33"/>
-      <c r="M11" s="33"/>
-      <c r="N11" s="33"/>
-      <c r="O11" s="33"/>
-      <c r="P11" s="33"/>
-      <c r="Q11" s="33"/>
-      <c r="R11" s="33"/>
-      <c r="S11" s="33"/>
-      <c r="T11" s="33"/>
-      <c r="U11" s="33"/>
-      <c r="V11" s="33"/>
-      <c r="W11" s="33"/>
-      <c r="X11" s="33"/>
-      <c r="Y11" s="33"/>
-      <c r="Z11" s="33"/>
-      <c r="AA11" s="33"/>
-      <c r="AB11" s="33"/>
-      <c r="AC11" s="33"/>
-      <c r="AD11" s="33"/>
-      <c r="AE11" s="33"/>
-      <c r="AF11" s="33"/>
-      <c r="AG11" s="33"/>
-      <c r="AH11" s="33"/>
-      <c r="AI11" s="33"/>
-      <c r="AJ11" s="33"/>
-      <c r="AK11" s="33"/>
-      <c r="AL11" s="33"/>
-      <c r="AM11" s="33"/>
-      <c r="AN11" s="33"/>
-      <c r="AO11" s="33"/>
-      <c r="AP11" s="33"/>
-      <c r="AQ11" s="33"/>
-      <c r="AR11" s="33"/>
-      <c r="AS11" s="35"/>
-      <c r="AT11" s="13" t="s">
+      <c r="AU11" s="13" t="s">
         <v>485</v>
       </c>
-      <c r="AU11" s="13" t="s">
+      <c r="AV11" s="13" t="s">
         <v>486</v>
       </c>
-      <c r="AV11" s="13" t="s">
+      <c r="AW11" s="12" t="s">
         <v>487</v>
       </c>
-      <c r="AW11" s="12" t="s">
+      <c r="AX11" s="12" t="s">
         <v>488</v>
       </c>
-      <c r="AX11" s="12" t="s">
+      <c r="AY11" s="12" t="s">
         <v>489</v>
       </c>
-      <c r="AY11" s="12" t="s">
+      <c r="AZ11" s="12" t="s">
         <v>490</v>
       </c>
-      <c r="AZ11" s="12" t="s">
+      <c r="BA11" s="12" t="s">
         <v>491</v>
       </c>
-      <c r="BA11" s="12" t="s">
+      <c r="BB11" s="12" t="s">
         <v>492</v>
       </c>
-      <c r="BB11" s="12" t="s">
+      <c r="BC11" s="12" t="s">
         <v>493</v>
       </c>
-      <c r="BC11" s="12" t="s">
+      <c r="BD11" s="12" t="s">
         <v>494</v>
       </c>
-      <c r="BD11" s="12" t="s">
+      <c r="BE11" s="12" t="s">
         <v>495</v>
       </c>
-      <c r="BE11" s="12" t="s">
+      <c r="BF11" s="12" t="s">
         <v>496</v>
       </c>
-      <c r="BF11" s="12" t="s">
+      <c r="BG11" s="12" t="s">
         <v>497</v>
       </c>
-      <c r="BG11" s="12" t="s">
+      <c r="BH11" s="12" t="s">
         <v>498</v>
       </c>
-      <c r="BH11" s="12" t="s">
+      <c r="BI11" s="18" t="s">
         <v>499</v>
       </c>
-      <c r="BI11" s="18" t="s">
-        <v>500</v>
-      </c>
-      <c r="BJ11" s="31"/>
-      <c r="BK11" s="29"/>
-      <c r="BL11" s="29"/>
-      <c r="BM11" s="29"/>
+      <c r="BJ11" s="36"/>
+      <c r="BK11" s="32"/>
+      <c r="BL11" s="32"/>
+      <c r="BM11" s="32"/>
     </row>
     <row r="12" spans="1:65" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="29"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="30">
+      <c r="A12" s="32"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="33">
         <v>4</v>
       </c>
       <c r="F12" s="4">
@@ -17729,17 +17749,17 @@
       <c r="BI12" s="3">
         <v>100</v>
       </c>
-      <c r="BJ12" s="31"/>
-      <c r="BK12" s="29"/>
-      <c r="BL12" s="29"/>
-      <c r="BM12" s="29"/>
+      <c r="BJ12" s="36"/>
+      <c r="BK12" s="32"/>
+      <c r="BL12" s="32"/>
+      <c r="BM12" s="32"/>
     </row>
     <row r="13" spans="1:65" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="29"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="30"/>
+      <c r="A13" s="32"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="33"/>
       <c r="F13" s="8" t="s">
         <v>42</v>
       </c>
@@ -17777,13 +17797,13 @@
         <v>123</v>
       </c>
       <c r="R13" s="8" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="S13" s="8" t="s">
         <v>124</v>
       </c>
       <c r="T13" s="8" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="U13" s="8" t="s">
         <v>125</v>
@@ -17795,19 +17815,19 @@
         <v>127</v>
       </c>
       <c r="X13" s="8" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="Y13" s="8" t="s">
         <v>128</v>
       </c>
       <c r="Z13" s="8" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="AA13" s="8" t="s">
         <v>129</v>
       </c>
       <c r="AB13" s="8" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="AC13" s="8" t="s">
         <v>130</v>
@@ -17828,7 +17848,7 @@
         <v>135</v>
       </c>
       <c r="AI13" s="8" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="AJ13" s="8" t="s">
         <v>136</v>
@@ -17843,7 +17863,7 @@
         <v>139</v>
       </c>
       <c r="AN13" s="8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="AO13" s="8" t="s">
         <v>142</v>
@@ -17908,196 +17928,196 @@
       <c r="BI13" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="BJ13" s="31"/>
-      <c r="BK13" s="29"/>
-      <c r="BL13" s="29"/>
-      <c r="BM13" s="29"/>
+      <c r="BJ13" s="36"/>
+      <c r="BK13" s="32"/>
+      <c r="BL13" s="32"/>
+      <c r="BM13" s="32"/>
     </row>
     <row r="14" spans="1:65" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="29"/>
-      <c r="B14" s="29"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="30"/>
+      <c r="A14" s="32"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="33"/>
       <c r="F14" s="13" t="s">
+        <v>500</v>
+      </c>
+      <c r="G14" s="13" t="s">
         <v>501</v>
       </c>
-      <c r="G14" s="13" t="s">
+      <c r="H14" s="13" t="s">
         <v>502</v>
       </c>
-      <c r="H14" s="13" t="s">
+      <c r="I14" s="13" t="s">
         <v>503</v>
       </c>
-      <c r="I14" s="13" t="s">
+      <c r="J14" s="13" t="s">
         <v>504</v>
       </c>
-      <c r="J14" s="13" t="s">
+      <c r="K14" s="13" t="s">
         <v>505</v>
       </c>
-      <c r="K14" s="13" t="s">
+      <c r="L14" s="13" t="s">
         <v>506</v>
       </c>
-      <c r="L14" s="13" t="s">
+      <c r="M14" s="13" t="s">
         <v>507</v>
       </c>
-      <c r="M14" s="13" t="s">
+      <c r="N14" s="13" t="s">
         <v>508</v>
       </c>
-      <c r="N14" s="13" t="s">
+      <c r="O14" s="13" t="s">
         <v>509</v>
       </c>
-      <c r="O14" s="13" t="s">
+      <c r="P14" s="13" t="s">
         <v>510</v>
       </c>
-      <c r="P14" s="13" t="s">
+      <c r="Q14" s="13" t="s">
         <v>511</v>
       </c>
-      <c r="Q14" s="13" t="s">
+      <c r="R14" s="13" t="s">
         <v>512</v>
       </c>
-      <c r="R14" s="13" t="s">
+      <c r="S14" s="13" t="s">
         <v>513</v>
       </c>
-      <c r="S14" s="13" t="s">
+      <c r="T14" s="13" t="s">
         <v>514</v>
       </c>
-      <c r="T14" s="13" t="s">
+      <c r="U14" s="13" t="s">
         <v>515</v>
       </c>
-      <c r="U14" s="13" t="s">
+      <c r="V14" s="13" t="s">
         <v>516</v>
       </c>
-      <c r="V14" s="13" t="s">
+      <c r="W14" s="13" t="s">
         <v>517</v>
       </c>
-      <c r="W14" s="13" t="s">
+      <c r="X14" s="13" t="s">
         <v>518</v>
       </c>
-      <c r="X14" s="13" t="s">
+      <c r="Y14" s="13" t="s">
         <v>519</v>
       </c>
-      <c r="Y14" s="13" t="s">
+      <c r="Z14" s="13" t="s">
         <v>520</v>
       </c>
-      <c r="Z14" s="13" t="s">
+      <c r="AA14" s="13" t="s">
         <v>521</v>
       </c>
-      <c r="AA14" s="13" t="s">
+      <c r="AB14" s="13" t="s">
         <v>522</v>
       </c>
-      <c r="AB14" s="13" t="s">
+      <c r="AC14" s="13" t="s">
         <v>523</v>
       </c>
-      <c r="AC14" s="13" t="s">
+      <c r="AD14" s="13" t="s">
         <v>524</v>
       </c>
-      <c r="AD14" s="13" t="s">
+      <c r="AE14" s="13" t="s">
         <v>525</v>
       </c>
-      <c r="AE14" s="13" t="s">
+      <c r="AF14" s="13" t="s">
         <v>526</v>
       </c>
-      <c r="AF14" s="13" t="s">
+      <c r="AG14" s="13" t="s">
         <v>527</v>
       </c>
-      <c r="AG14" s="13" t="s">
+      <c r="AH14" s="13" t="s">
         <v>528</v>
       </c>
-      <c r="AH14" s="13" t="s">
+      <c r="AI14" s="13" t="s">
         <v>529</v>
       </c>
-      <c r="AI14" s="13" t="s">
+      <c r="AJ14" s="13" t="s">
         <v>530</v>
       </c>
-      <c r="AJ14" s="13" t="s">
+      <c r="AK14" s="13" t="s">
         <v>531</v>
       </c>
-      <c r="AK14" s="13" t="s">
+      <c r="AL14" s="13" t="s">
         <v>532</v>
       </c>
-      <c r="AL14" s="13" t="s">
+      <c r="AM14" s="13" t="s">
         <v>533</v>
       </c>
-      <c r="AM14" s="13" t="s">
+      <c r="AN14" s="13" t="s">
         <v>534</v>
       </c>
-      <c r="AN14" s="13" t="s">
+      <c r="AO14" s="13" t="s">
         <v>535</v>
       </c>
-      <c r="AO14" s="13" t="s">
+      <c r="AP14" s="13" t="s">
         <v>536</v>
       </c>
-      <c r="AP14" s="13" t="s">
+      <c r="AQ14" s="13" t="s">
         <v>537</v>
       </c>
-      <c r="AQ14" s="13" t="s">
+      <c r="AR14" s="13" t="s">
         <v>538</v>
       </c>
-      <c r="AR14" s="13" t="s">
+      <c r="AS14" s="13" t="s">
         <v>539</v>
       </c>
-      <c r="AS14" s="13" t="s">
+      <c r="AT14" s="13" t="s">
         <v>540</v>
       </c>
-      <c r="AT14" s="13" t="s">
+      <c r="AU14" s="13" t="s">
         <v>541</v>
       </c>
-      <c r="AU14" s="13" t="s">
+      <c r="AV14" s="13" t="s">
         <v>542</v>
       </c>
-      <c r="AV14" s="13" t="s">
+      <c r="AW14" s="13" t="s">
         <v>543</v>
       </c>
-      <c r="AW14" s="13" t="s">
+      <c r="AX14" s="13" t="s">
         <v>544</v>
       </c>
-      <c r="AX14" s="13" t="s">
+      <c r="AY14" s="13" t="s">
         <v>545</v>
       </c>
-      <c r="AY14" s="13" t="s">
+      <c r="AZ14" s="12" t="s">
         <v>546</v>
       </c>
-      <c r="AZ14" s="12" t="s">
+      <c r="BA14" s="12" t="s">
         <v>547</v>
       </c>
-      <c r="BA14" s="12" t="s">
+      <c r="BB14" s="12" t="s">
         <v>548</v>
       </c>
-      <c r="BB14" s="12" t="s">
+      <c r="BC14" s="12" t="s">
         <v>549</v>
       </c>
-      <c r="BC14" s="12" t="s">
+      <c r="BD14" s="12" t="s">
         <v>550</v>
       </c>
-      <c r="BD14" s="12" t="s">
+      <c r="BE14" s="12" t="s">
         <v>551</v>
       </c>
-      <c r="BE14" s="12" t="s">
+      <c r="BF14" s="12" t="s">
         <v>552</v>
       </c>
-      <c r="BF14" s="12" t="s">
+      <c r="BG14" s="12" t="s">
         <v>553</v>
       </c>
-      <c r="BG14" s="12" t="s">
+      <c r="BH14" s="12" t="s">
         <v>554</v>
       </c>
-      <c r="BH14" s="12" t="s">
+      <c r="BI14" s="18" t="s">
         <v>555</v>
       </c>
-      <c r="BI14" s="18" t="s">
-        <v>556</v>
-      </c>
-      <c r="BJ14" s="31"/>
-      <c r="BK14" s="29"/>
-      <c r="BL14" s="29"/>
-      <c r="BM14" s="29"/>
+      <c r="BJ14" s="36"/>
+      <c r="BK14" s="32"/>
+      <c r="BL14" s="32"/>
+      <c r="BM14" s="32"/>
     </row>
     <row r="15" spans="1:65" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="29"/>
-      <c r="B15" s="29"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="30">
+      <c r="A15" s="32"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="33">
         <v>5</v>
       </c>
       <c r="F15" s="4">
@@ -18268,17 +18288,17 @@
       <c r="BI15" s="3">
         <v>156</v>
       </c>
-      <c r="BJ15" s="31"/>
-      <c r="BK15" s="29"/>
-      <c r="BL15" s="29"/>
-      <c r="BM15" s="29"/>
+      <c r="BJ15" s="36"/>
+      <c r="BK15" s="32"/>
+      <c r="BL15" s="32"/>
+      <c r="BM15" s="32"/>
     </row>
     <row r="16" spans="1:65" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="29"/>
-      <c r="B16" s="29"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="30"/>
+      <c r="A16" s="32"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="33"/>
       <c r="F16" s="8" t="s">
         <v>62</v>
       </c>
@@ -18292,7 +18312,7 @@
         <v>65</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K16" s="8" t="s">
         <v>145</v>
@@ -18322,7 +18342,7 @@
         <v>153</v>
       </c>
       <c r="T16" s="8" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="U16" s="8" t="s">
         <v>154</v>
@@ -18367,7 +18387,7 @@
         <v>167</v>
       </c>
       <c r="AI16" s="8" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="AJ16" s="8" t="s">
         <v>168</v>
@@ -18394,13 +18414,13 @@
         <v>173</v>
       </c>
       <c r="AR16" s="8" t="s">
+        <v>854</v>
+      </c>
+      <c r="AS16" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="AS16" s="8" t="s">
-        <v>177</v>
-      </c>
       <c r="AT16" s="8" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="AU16" s="8" t="s">
         <v>66</v>
@@ -18418,7 +18438,7 @@
         <v>70</v>
       </c>
       <c r="AZ16" s="8" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="BA16" s="8" t="s">
         <v>71</v>
@@ -18447,196 +18467,196 @@
       <c r="BI16" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="BJ16" s="31"/>
-      <c r="BK16" s="29"/>
-      <c r="BL16" s="29"/>
-      <c r="BM16" s="29"/>
+      <c r="BJ16" s="36"/>
+      <c r="BK16" s="32"/>
+      <c r="BL16" s="32"/>
+      <c r="BM16" s="32"/>
     </row>
     <row r="17" spans="1:65" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="30"/>
+      <c r="A17" s="32"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="33"/>
       <c r="F17" s="13" t="s">
+        <v>556</v>
+      </c>
+      <c r="G17" s="13" t="s">
         <v>557</v>
       </c>
-      <c r="G17" s="13" t="s">
+      <c r="H17" s="13" t="s">
         <v>558</v>
       </c>
-      <c r="H17" s="13" t="s">
+      <c r="I17" s="13" t="s">
         <v>559</v>
       </c>
-      <c r="I17" s="13" t="s">
+      <c r="J17" s="13" t="s">
         <v>560</v>
       </c>
-      <c r="J17" s="13" t="s">
+      <c r="K17" s="13" t="s">
         <v>561</v>
       </c>
-      <c r="K17" s="13" t="s">
+      <c r="L17" s="13" t="s">
         <v>562</v>
       </c>
-      <c r="L17" s="13" t="s">
+      <c r="M17" s="13" t="s">
         <v>563</v>
       </c>
-      <c r="M17" s="13" t="s">
+      <c r="N17" s="13" t="s">
         <v>564</v>
       </c>
-      <c r="N17" s="13" t="s">
+      <c r="O17" s="13" t="s">
         <v>565</v>
       </c>
-      <c r="O17" s="13" t="s">
+      <c r="P17" s="13" t="s">
         <v>566</v>
       </c>
-      <c r="P17" s="13" t="s">
+      <c r="Q17" s="13" t="s">
         <v>567</v>
       </c>
-      <c r="Q17" s="13" t="s">
+      <c r="R17" s="13" t="s">
         <v>568</v>
       </c>
-      <c r="R17" s="13" t="s">
+      <c r="S17" s="13" t="s">
         <v>569</v>
       </c>
-      <c r="S17" s="13" t="s">
+      <c r="T17" s="13" t="s">
         <v>570</v>
       </c>
-      <c r="T17" s="13" t="s">
+      <c r="U17" s="13" t="s">
         <v>571</v>
       </c>
-      <c r="U17" s="13" t="s">
+      <c r="V17" s="13" t="s">
         <v>572</v>
       </c>
-      <c r="V17" s="13" t="s">
+      <c r="W17" s="13" t="s">
         <v>573</v>
       </c>
-      <c r="W17" s="13" t="s">
+      <c r="X17" s="13" t="s">
         <v>574</v>
       </c>
-      <c r="X17" s="13" t="s">
+      <c r="Y17" s="13" t="s">
         <v>575</v>
       </c>
-      <c r="Y17" s="13" t="s">
+      <c r="Z17" s="13" t="s">
         <v>576</v>
       </c>
-      <c r="Z17" s="13" t="s">
+      <c r="AA17" s="13" t="s">
         <v>577</v>
       </c>
-      <c r="AA17" s="13" t="s">
+      <c r="AB17" s="13" t="s">
         <v>578</v>
       </c>
-      <c r="AB17" s="13" t="s">
+      <c r="AC17" s="13" t="s">
         <v>579</v>
       </c>
-      <c r="AC17" s="13" t="s">
+      <c r="AD17" s="13" t="s">
         <v>580</v>
       </c>
-      <c r="AD17" s="13" t="s">
+      <c r="AE17" s="13" t="s">
         <v>581</v>
       </c>
-      <c r="AE17" s="13" t="s">
+      <c r="AF17" s="13" t="s">
         <v>582</v>
       </c>
-      <c r="AF17" s="13" t="s">
+      <c r="AG17" s="13" t="s">
         <v>583</v>
       </c>
-      <c r="AG17" s="13" t="s">
+      <c r="AH17" s="13" t="s">
         <v>584</v>
       </c>
-      <c r="AH17" s="13" t="s">
+      <c r="AI17" s="13" t="s">
         <v>585</v>
       </c>
-      <c r="AI17" s="13" t="s">
+      <c r="AJ17" s="13" t="s">
         <v>586</v>
       </c>
-      <c r="AJ17" s="13" t="s">
+      <c r="AK17" s="13" t="s">
         <v>587</v>
       </c>
-      <c r="AK17" s="13" t="s">
+      <c r="AL17" s="13" t="s">
         <v>588</v>
       </c>
-      <c r="AL17" s="13" t="s">
+      <c r="AM17" s="13" t="s">
         <v>589</v>
       </c>
-      <c r="AM17" s="13" t="s">
+      <c r="AN17" s="13" t="s">
         <v>590</v>
       </c>
-      <c r="AN17" s="13" t="s">
+      <c r="AO17" s="13" t="s">
         <v>591</v>
       </c>
-      <c r="AO17" s="13" t="s">
+      <c r="AP17" s="13" t="s">
         <v>592</v>
       </c>
-      <c r="AP17" s="13" t="s">
+      <c r="AQ17" s="13" t="s">
         <v>593</v>
       </c>
-      <c r="AQ17" s="13" t="s">
+      <c r="AR17" s="13" t="s">
         <v>594</v>
       </c>
-      <c r="AR17" s="13" t="s">
+      <c r="AS17" s="13" t="s">
         <v>595</v>
       </c>
-      <c r="AS17" s="13" t="s">
+      <c r="AT17" s="13" t="s">
         <v>596</v>
       </c>
-      <c r="AT17" s="13" t="s">
+      <c r="AU17" s="13" t="s">
         <v>597</v>
       </c>
-      <c r="AU17" s="13" t="s">
+      <c r="AV17" s="13" t="s">
         <v>598</v>
       </c>
-      <c r="AV17" s="13" t="s">
+      <c r="AW17" s="13" t="s">
         <v>599</v>
       </c>
-      <c r="AW17" s="13" t="s">
+      <c r="AX17" s="13" t="s">
         <v>600</v>
       </c>
-      <c r="AX17" s="13" t="s">
+      <c r="AY17" s="13" t="s">
         <v>601</v>
       </c>
-      <c r="AY17" s="13" t="s">
+      <c r="AZ17" s="13" t="s">
         <v>602</v>
       </c>
-      <c r="AZ17" s="13" t="s">
+      <c r="BA17" s="13" t="s">
         <v>603</v>
       </c>
-      <c r="BA17" s="13" t="s">
+      <c r="BB17" s="13" t="s">
         <v>604</v>
       </c>
-      <c r="BB17" s="13" t="s">
+      <c r="BC17" s="12" t="s">
         <v>605</v>
       </c>
-      <c r="BC17" s="12" t="s">
+      <c r="BD17" s="12" t="s">
         <v>606</v>
       </c>
-      <c r="BD17" s="12" t="s">
+      <c r="BE17" s="12" t="s">
         <v>607</v>
       </c>
-      <c r="BE17" s="12" t="s">
+      <c r="BF17" s="12" t="s">
         <v>608</v>
       </c>
-      <c r="BF17" s="12" t="s">
+      <c r="BG17" s="12" t="s">
         <v>609</v>
       </c>
-      <c r="BG17" s="12" t="s">
+      <c r="BH17" s="12" t="s">
         <v>610</v>
       </c>
-      <c r="BH17" s="12" t="s">
+      <c r="BI17" s="18" t="s">
         <v>611</v>
       </c>
-      <c r="BI17" s="18" t="s">
-        <v>612</v>
-      </c>
-      <c r="BJ17" s="31"/>
-      <c r="BK17" s="29"/>
-      <c r="BL17" s="29"/>
-      <c r="BM17" s="29"/>
+      <c r="BJ17" s="36"/>
+      <c r="BK17" s="32"/>
+      <c r="BL17" s="32"/>
+      <c r="BM17" s="32"/>
     </row>
     <row r="18" spans="1:65" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="30">
+      <c r="A18" s="32"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="33">
         <v>6</v>
       </c>
       <c r="F18" s="4">
@@ -18807,17 +18827,17 @@
       <c r="BI18" s="3">
         <v>276</v>
       </c>
-      <c r="BJ18" s="31"/>
-      <c r="BK18" s="29"/>
-      <c r="BL18" s="29"/>
-      <c r="BM18" s="29"/>
+      <c r="BJ18" s="36"/>
+      <c r="BK18" s="32"/>
+      <c r="BL18" s="32"/>
+      <c r="BM18" s="32"/>
     </row>
     <row r="19" spans="1:65" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="29"/>
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="30"/>
+      <c r="A19" s="32"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="33"/>
       <c r="F19" s="8" t="s">
         <v>80</v>
       </c>
@@ -18831,112 +18851,112 @@
         <v>83</v>
       </c>
       <c r="J19" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="K19" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="K19" s="8" t="s">
+      <c r="L19" s="8" t="s">
+        <v>450</v>
+      </c>
+      <c r="M19" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="L19" s="8" t="s">
+      <c r="N19" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="O19" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="P19" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q19" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="R19" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="S19" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="T19" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="U19" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="V19" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="W19" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="X19" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="Y19" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="Z19" s="8" t="s">
         <v>451</v>
       </c>
-      <c r="M19" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="N19" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="O19" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="P19" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="Q19" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="R19" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="S19" s="8" t="s">
-        <v>186</v>
-      </c>
-      <c r="T19" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="U19" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="V19" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="W19" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="X19" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="Y19" s="8" t="s">
+      <c r="AA19" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="Z19" s="8" t="s">
+      <c r="AB19" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="AC19" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="AD19" s="8" t="s">
+        <v>415</v>
+      </c>
+      <c r="AE19" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="AF19" s="8" t="s">
+        <v>416</v>
+      </c>
+      <c r="AG19" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="AH19" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="AI19" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="AJ19" s="8" t="s">
         <v>452</v>
       </c>
-      <c r="AA19" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="AB19" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="AC19" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="AD19" s="8" t="s">
-        <v>416</v>
-      </c>
-      <c r="AE19" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="AF19" s="8" t="s">
-        <v>417</v>
-      </c>
-      <c r="AG19" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="AH19" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="AI19" s="8" t="s">
+      <c r="AK19" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="AJ19" s="8" t="s">
-        <v>453</v>
-      </c>
-      <c r="AK19" s="8" t="s">
+      <c r="AL19" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="AL19" s="8" t="s">
+      <c r="AM19" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="AM19" s="8" t="s">
+      <c r="AN19" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="AN19" s="8" t="s">
+      <c r="AO19" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="AP19" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="AQ19" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="AO19" s="8" t="s">
+      <c r="AR19" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="AP19" s="8" t="s">
-        <v>205</v>
-      </c>
-      <c r="AQ19" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="AR19" s="8" t="s">
+      <c r="AS19" s="8" t="s">
         <v>207</v>
-      </c>
-      <c r="AS19" s="8" t="s">
-        <v>208</v>
       </c>
       <c r="AT19" s="8" t="s">
         <v>84</v>
@@ -18986,196 +19006,196 @@
       <c r="BI19" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="BJ19" s="31"/>
-      <c r="BK19" s="29"/>
-      <c r="BL19" s="29"/>
-      <c r="BM19" s="29"/>
+      <c r="BJ19" s="36"/>
+      <c r="BK19" s="32"/>
+      <c r="BL19" s="32"/>
+      <c r="BM19" s="32"/>
     </row>
     <row r="20" spans="1:65" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="29"/>
-      <c r="B20" s="29"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="30"/>
+      <c r="A20" s="32"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="33"/>
       <c r="F20" s="13" t="s">
+        <v>612</v>
+      </c>
+      <c r="G20" s="13" t="s">
         <v>613</v>
       </c>
-      <c r="G20" s="13" t="s">
+      <c r="H20" s="13" t="s">
         <v>614</v>
       </c>
-      <c r="H20" s="13" t="s">
+      <c r="I20" s="13" t="s">
         <v>615</v>
       </c>
-      <c r="I20" s="13" t="s">
+      <c r="J20" s="14" t="s">
         <v>616</v>
       </c>
-      <c r="J20" s="14" t="s">
+      <c r="K20" s="13" t="s">
         <v>617</v>
       </c>
-      <c r="K20" s="13" t="s">
+      <c r="L20" s="13" t="s">
         <v>618</v>
       </c>
-      <c r="L20" s="13" t="s">
+      <c r="M20" s="13" t="s">
         <v>619</v>
       </c>
-      <c r="M20" s="13" t="s">
+      <c r="N20" s="13" t="s">
         <v>620</v>
       </c>
-      <c r="N20" s="13" t="s">
+      <c r="O20" s="13" t="s">
         <v>621</v>
       </c>
-      <c r="O20" s="13" t="s">
+      <c r="P20" s="13" t="s">
         <v>622</v>
       </c>
-      <c r="P20" s="13" t="s">
+      <c r="Q20" s="13" t="s">
         <v>623</v>
       </c>
-      <c r="Q20" s="13" t="s">
+      <c r="R20" s="13" t="s">
         <v>624</v>
       </c>
-      <c r="R20" s="13" t="s">
+      <c r="S20" s="13" t="s">
         <v>625</v>
       </c>
-      <c r="S20" s="13" t="s">
+      <c r="T20" s="13" t="s">
         <v>626</v>
       </c>
-      <c r="T20" s="13" t="s">
+      <c r="U20" s="13" t="s">
         <v>627</v>
       </c>
-      <c r="U20" s="13" t="s">
+      <c r="V20" s="13" t="s">
         <v>628</v>
       </c>
-      <c r="V20" s="13" t="s">
+      <c r="W20" s="13" t="s">
         <v>629</v>
       </c>
-      <c r="W20" s="13" t="s">
+      <c r="X20" s="13" t="s">
         <v>630</v>
       </c>
-      <c r="X20" s="13" t="s">
+      <c r="Y20" s="13" t="s">
         <v>631</v>
       </c>
-      <c r="Y20" s="13" t="s">
+      <c r="Z20" s="13" t="s">
         <v>632</v>
       </c>
-      <c r="Z20" s="13" t="s">
+      <c r="AA20" s="13" t="s">
         <v>633</v>
       </c>
-      <c r="AA20" s="13" t="s">
+      <c r="AB20" s="13" t="s">
         <v>634</v>
       </c>
-      <c r="AB20" s="13" t="s">
+      <c r="AC20" s="13" t="s">
         <v>635</v>
       </c>
-      <c r="AC20" s="13" t="s">
+      <c r="AD20" s="13" t="s">
         <v>636</v>
       </c>
-      <c r="AD20" s="13" t="s">
+      <c r="AE20" s="13" t="s">
         <v>637</v>
       </c>
-      <c r="AE20" s="13" t="s">
+      <c r="AF20" s="13" t="s">
         <v>638</v>
       </c>
-      <c r="AF20" s="13" t="s">
+      <c r="AG20" s="13" t="s">
         <v>639</v>
       </c>
-      <c r="AG20" s="13" t="s">
+      <c r="AH20" s="13" t="s">
         <v>640</v>
       </c>
-      <c r="AH20" s="13" t="s">
+      <c r="AI20" s="13" t="s">
         <v>641</v>
       </c>
-      <c r="AI20" s="13" t="s">
+      <c r="AJ20" s="13" t="s">
         <v>642</v>
       </c>
-      <c r="AJ20" s="13" t="s">
+      <c r="AK20" s="13" t="s">
         <v>643</v>
       </c>
-      <c r="AK20" s="13" t="s">
+      <c r="AL20" s="13" t="s">
         <v>644</v>
       </c>
-      <c r="AL20" s="13" t="s">
+      <c r="AM20" s="13" t="s">
         <v>645</v>
       </c>
-      <c r="AM20" s="13" t="s">
+      <c r="AN20" s="13" t="s">
         <v>646</v>
       </c>
-      <c r="AN20" s="13" t="s">
+      <c r="AO20" s="13" t="s">
         <v>647</v>
       </c>
-      <c r="AO20" s="13" t="s">
+      <c r="AP20" s="13" t="s">
         <v>648</v>
       </c>
-      <c r="AP20" s="13" t="s">
+      <c r="AQ20" s="13" t="s">
         <v>649</v>
       </c>
-      <c r="AQ20" s="13" t="s">
+      <c r="AR20" s="13" t="s">
         <v>650</v>
       </c>
-      <c r="AR20" s="13" t="s">
+      <c r="AS20" s="13" t="s">
         <v>651</v>
       </c>
-      <c r="AS20" s="13" t="s">
+      <c r="AT20" s="13" t="s">
         <v>652</v>
       </c>
-      <c r="AT20" s="13" t="s">
+      <c r="AU20" s="13" t="s">
         <v>653</v>
       </c>
-      <c r="AU20" s="13" t="s">
+      <c r="AV20" s="13" t="s">
         <v>654</v>
       </c>
-      <c r="AV20" s="13" t="s">
+      <c r="AW20" s="13" t="s">
         <v>655</v>
       </c>
-      <c r="AW20" s="13" t="s">
+      <c r="AX20" s="13" t="s">
         <v>656</v>
       </c>
-      <c r="AX20" s="13" t="s">
+      <c r="AY20" s="13" t="s">
         <v>657</v>
       </c>
-      <c r="AY20" s="13" t="s">
+      <c r="AZ20" s="13" t="s">
         <v>658</v>
       </c>
-      <c r="AZ20" s="13" t="s">
+      <c r="BA20" s="13" t="s">
         <v>659</v>
       </c>
-      <c r="BA20" s="13" t="s">
+      <c r="BB20" s="13" t="s">
         <v>660</v>
       </c>
-      <c r="BB20" s="13" t="s">
+      <c r="BC20" s="13" t="s">
         <v>661</v>
       </c>
-      <c r="BC20" s="13" t="s">
+      <c r="BD20" s="13" t="s">
         <v>662</v>
       </c>
-      <c r="BD20" s="13" t="s">
+      <c r="BE20" s="13" t="s">
         <v>663</v>
       </c>
-      <c r="BE20" s="13" t="s">
+      <c r="BF20" s="12" t="s">
         <v>664</v>
       </c>
-      <c r="BF20" s="12" t="s">
+      <c r="BG20" s="12" t="s">
         <v>665</v>
       </c>
-      <c r="BG20" s="12" t="s">
+      <c r="BH20" s="12" t="s">
         <v>666</v>
       </c>
-      <c r="BH20" s="12" t="s">
+      <c r="BI20" s="18" t="s">
         <v>667</v>
       </c>
-      <c r="BI20" s="18" t="s">
-        <v>668</v>
-      </c>
-      <c r="BJ20" s="31"/>
-      <c r="BK20" s="29"/>
-      <c r="BL20" s="29"/>
-      <c r="BM20" s="29"/>
+      <c r="BJ20" s="36"/>
+      <c r="BK20" s="32"/>
+      <c r="BL20" s="32"/>
+      <c r="BM20" s="32"/>
     </row>
     <row r="21" spans="1:65" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="29"/>
-      <c r="B21" s="29"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="30">
+      <c r="A21" s="32"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="33">
         <v>7</v>
       </c>
       <c r="F21" s="4">
@@ -19346,136 +19366,136 @@
       <c r="BI21" s="3">
         <v>396</v>
       </c>
-      <c r="BJ21" s="31"/>
-      <c r="BK21" s="29"/>
-      <c r="BL21" s="29"/>
-      <c r="BM21" s="29"/>
+      <c r="BJ21" s="36"/>
+      <c r="BK21" s="32"/>
+      <c r="BL21" s="32"/>
+      <c r="BM21" s="32"/>
     </row>
     <row r="22" spans="1:65" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="29"/>
-      <c r="B22" s="29"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="30"/>
+      <c r="A22" s="32"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="33"/>
       <c r="F22" s="8" t="s">
         <v>100</v>
       </c>
       <c r="G22" s="8" t="s">
+        <v>436</v>
+      </c>
+      <c r="H22" s="8" t="s">
         <v>437</v>
-      </c>
-      <c r="H22" s="8" t="s">
-        <v>438</v>
       </c>
       <c r="I22" s="8" t="s">
         <v>101</v>
       </c>
       <c r="J22" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="K22" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="K22" s="8" t="s">
+      <c r="L22" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="L22" s="8" t="s">
+      <c r="M22" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="M22" s="8" t="s">
+      <c r="N22" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="N22" s="8" t="s">
+      <c r="O22" s="8" t="s">
+        <v>849</v>
+      </c>
+      <c r="P22" s="8" t="s">
+        <v>453</v>
+      </c>
+      <c r="Q22" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="O22" s="8" t="s">
-        <v>850</v>
-      </c>
-      <c r="P22" s="8" t="s">
-        <v>454</v>
-      </c>
-      <c r="Q22" s="8" t="s">
+      <c r="R22" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="R22" s="8" t="s">
+      <c r="S22" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="S22" s="8" t="s">
+      <c r="T22" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="T22" s="8" t="s">
+      <c r="U22" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="U22" s="8" t="s">
+      <c r="V22" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="W22" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="V22" s="8" t="s">
+      <c r="X22" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="Y22" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="Z22" s="8" t="s">
         <v>418</v>
       </c>
-      <c r="W22" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="X22" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="Y22" s="8" t="s">
+      <c r="AA22" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="Z22" s="8" t="s">
+      <c r="AB22" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="AC22" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD22" s="8" t="s">
         <v>419</v>
       </c>
-      <c r="AA22" s="8" t="s">
-        <v>222</v>
-      </c>
-      <c r="AB22" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="AC22" s="8" t="s">
+      <c r="AE22" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="AD22" s="8" t="s">
+      <c r="AF22" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="AG22" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="AH22" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="AI22" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="AJ22" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="AK22" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="AL22" s="8" t="s">
         <v>420</v>
       </c>
-      <c r="AE22" s="8" t="s">
-        <v>225</v>
-      </c>
-      <c r="AF22" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="AG22" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="AH22" s="8" t="s">
-        <v>228</v>
-      </c>
-      <c r="AI22" s="8" t="s">
-        <v>229</v>
-      </c>
-      <c r="AJ22" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="AK22" s="8" t="s">
+      <c r="AM22" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="AL22" s="8" t="s">
+      <c r="AN22" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="AO22" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="AP22" s="8" t="s">
         <v>421</v>
       </c>
-      <c r="AM22" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="AN22" s="8" t="s">
+      <c r="AQ22" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="AO22" s="8" t="s">
+      <c r="AR22" s="8" t="s">
         <v>235</v>
       </c>
-      <c r="AP22" s="8" t="s">
-        <v>422</v>
-      </c>
-      <c r="AQ22" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="AR22" s="8" t="s">
+      <c r="AS22" s="8" t="s">
         <v>236</v>
-      </c>
-      <c r="AS22" s="8" t="s">
-        <v>237</v>
       </c>
       <c r="AT22" s="8" t="s">
         <v>102</v>
@@ -19496,7 +19516,7 @@
         <v>107</v>
       </c>
       <c r="AZ22" s="8" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="BA22" s="8" t="s">
         <v>108</v>
@@ -19517,7 +19537,7 @@
         <v>113</v>
       </c>
       <c r="BG22" s="8" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="BH22" s="8" t="s">
         <v>114</v>
@@ -19525,189 +19545,189 @@
       <c r="BI22" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="BJ22" s="31"/>
-      <c r="BK22" s="29"/>
-      <c r="BL22" s="29"/>
-      <c r="BM22" s="29"/>
+      <c r="BJ22" s="36"/>
+      <c r="BK22" s="32"/>
+      <c r="BL22" s="32"/>
+      <c r="BM22" s="32"/>
     </row>
     <row r="23" spans="1:65" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="29"/>
-      <c r="B23" s="29"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="30"/>
+      <c r="A23" s="32"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="33"/>
       <c r="F23" s="13" t="s">
+        <v>668</v>
+      </c>
+      <c r="G23" s="13" t="s">
         <v>669</v>
       </c>
-      <c r="G23" s="13" t="s">
+      <c r="H23" s="13" t="s">
         <v>670</v>
       </c>
-      <c r="H23" s="13" t="s">
+      <c r="I23" s="13" t="s">
         <v>671</v>
       </c>
-      <c r="I23" s="13" t="s">
+      <c r="J23" s="14" t="s">
         <v>672</v>
       </c>
-      <c r="J23" s="14" t="s">
+      <c r="K23" s="13" t="s">
         <v>673</v>
       </c>
-      <c r="K23" s="13" t="s">
+      <c r="L23" s="13" t="s">
         <v>674</v>
       </c>
-      <c r="L23" s="13" t="s">
+      <c r="M23" s="13" t="s">
         <v>675</v>
       </c>
-      <c r="M23" s="13" t="s">
+      <c r="N23" s="13" t="s">
         <v>676</v>
       </c>
-      <c r="N23" s="13" t="s">
+      <c r="O23" s="13" t="s">
         <v>677</v>
       </c>
-      <c r="O23" s="13" t="s">
+      <c r="P23" s="13" t="s">
         <v>678</v>
       </c>
-      <c r="P23" s="13" t="s">
+      <c r="Q23" s="13" t="s">
         <v>679</v>
       </c>
-      <c r="Q23" s="13" t="s">
+      <c r="R23" s="13" t="s">
         <v>680</v>
       </c>
-      <c r="R23" s="13" t="s">
+      <c r="S23" s="13" t="s">
         <v>681</v>
       </c>
-      <c r="S23" s="13" t="s">
+      <c r="T23" s="13" t="s">
         <v>682</v>
       </c>
-      <c r="T23" s="13" t="s">
+      <c r="U23" s="13" t="s">
         <v>683</v>
       </c>
-      <c r="U23" s="13" t="s">
+      <c r="V23" s="13" t="s">
         <v>684</v>
       </c>
-      <c r="V23" s="13" t="s">
+      <c r="W23" s="13" t="s">
         <v>685</v>
       </c>
-      <c r="W23" s="13" t="s">
+      <c r="X23" s="13" t="s">
         <v>686</v>
       </c>
-      <c r="X23" s="13" t="s">
+      <c r="Y23" s="13" t="s">
         <v>687</v>
       </c>
-      <c r="Y23" s="13" t="s">
+      <c r="Z23" s="13" t="s">
         <v>688</v>
       </c>
-      <c r="Z23" s="13" t="s">
+      <c r="AA23" s="13" t="s">
         <v>689</v>
       </c>
-      <c r="AA23" s="13" t="s">
+      <c r="AB23" s="13" t="s">
         <v>690</v>
       </c>
-      <c r="AB23" s="13" t="s">
+      <c r="AC23" s="13" t="s">
         <v>691</v>
       </c>
-      <c r="AC23" s="13" t="s">
+      <c r="AD23" s="13" t="s">
         <v>692</v>
       </c>
-      <c r="AD23" s="13" t="s">
+      <c r="AE23" s="13" t="s">
         <v>693</v>
       </c>
-      <c r="AE23" s="13" t="s">
+      <c r="AF23" s="13" t="s">
         <v>694</v>
       </c>
-      <c r="AF23" s="13" t="s">
+      <c r="AG23" s="13" t="s">
         <v>695</v>
       </c>
-      <c r="AG23" s="13" t="s">
+      <c r="AH23" s="13" t="s">
         <v>696</v>
       </c>
-      <c r="AH23" s="13" t="s">
+      <c r="AI23" s="13" t="s">
         <v>697</v>
       </c>
-      <c r="AI23" s="13" t="s">
+      <c r="AJ23" s="13" t="s">
         <v>698</v>
       </c>
-      <c r="AJ23" s="13" t="s">
+      <c r="AK23" s="13" t="s">
         <v>699</v>
       </c>
-      <c r="AK23" s="13" t="s">
+      <c r="AL23" s="13" t="s">
         <v>700</v>
       </c>
-      <c r="AL23" s="13" t="s">
+      <c r="AM23" s="13" t="s">
         <v>701</v>
       </c>
-      <c r="AM23" s="13" t="s">
+      <c r="AN23" s="13" t="s">
         <v>702</v>
       </c>
-      <c r="AN23" s="13" t="s">
+      <c r="AO23" s="13" t="s">
         <v>703</v>
       </c>
-      <c r="AO23" s="13" t="s">
+      <c r="AP23" s="13" t="s">
+        <v>850</v>
+      </c>
+      <c r="AQ23" s="13" t="s">
+        <v>851</v>
+      </c>
+      <c r="AR23" s="13" t="s">
+        <v>852</v>
+      </c>
+      <c r="AS23" s="13" t="s">
+        <v>853</v>
+      </c>
+      <c r="AT23" s="13" t="s">
         <v>704</v>
       </c>
-      <c r="AP23" s="13" t="s">
-        <v>851</v>
-      </c>
-      <c r="AQ23" s="13" t="s">
-        <v>852</v>
-      </c>
-      <c r="AR23" s="13" t="s">
-        <v>853</v>
-      </c>
-      <c r="AS23" s="13" t="s">
-        <v>854</v>
-      </c>
-      <c r="AT23" s="13" t="s">
+      <c r="AU23" s="13" t="s">
         <v>705</v>
       </c>
-      <c r="AU23" s="13" t="s">
+      <c r="AV23" s="13" t="s">
         <v>706</v>
       </c>
-      <c r="AV23" s="13" t="s">
+      <c r="AW23" s="13" t="s">
         <v>707</v>
       </c>
-      <c r="AW23" s="13" t="s">
+      <c r="AX23" s="13" t="s">
         <v>708</v>
       </c>
-      <c r="AX23" s="13" t="s">
+      <c r="AY23" s="13" t="s">
         <v>709</v>
       </c>
-      <c r="AY23" s="13" t="s">
+      <c r="AZ23" s="13" t="s">
         <v>710</v>
       </c>
-      <c r="AZ23" s="13" t="s">
+      <c r="BA23" s="13" t="s">
         <v>711</v>
       </c>
-      <c r="BA23" s="13" t="s">
+      <c r="BB23" s="13" t="s">
         <v>712</v>
       </c>
-      <c r="BB23" s="13" t="s">
+      <c r="BC23" s="13" t="s">
         <v>713</v>
       </c>
-      <c r="BC23" s="13" t="s">
+      <c r="BD23" s="13" t="s">
         <v>714</v>
       </c>
-      <c r="BD23" s="13" t="s">
+      <c r="BE23" s="13" t="s">
         <v>715</v>
       </c>
-      <c r="BE23" s="13" t="s">
+      <c r="BF23" s="13" t="s">
         <v>716</v>
       </c>
-      <c r="BF23" s="13" t="s">
+      <c r="BG23" s="13" t="s">
         <v>717</v>
       </c>
-      <c r="BG23" s="13" t="s">
+      <c r="BH23" s="13" t="s">
         <v>718</v>
       </c>
-      <c r="BH23" s="13" t="s">
+      <c r="BI23" s="18" t="s">
         <v>719</v>
       </c>
-      <c r="BI23" s="18" t="s">
-        <v>720</v>
-      </c>
-      <c r="BJ23" s="31"/>
-      <c r="BK23" s="29"/>
-      <c r="BL23" s="29"/>
-      <c r="BM23" s="29"/>
+      <c r="BJ23" s="36"/>
+      <c r="BK23" s="32"/>
+      <c r="BL23" s="32"/>
+      <c r="BM23" s="32"/>
     </row>
     <row r="24" spans="1:65" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="11"/>
@@ -19777,8 +19797,8 @@
       <c r="BM24" s="11"/>
     </row>
     <row r="25" spans="1:65" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="30" t="s">
-        <v>439</v>
+      <c r="A25" s="33" t="s">
+        <v>438</v>
       </c>
       <c r="B25" s="6">
         <v>161</v>
@@ -19974,398 +19994,398 @@
       </c>
     </row>
     <row r="26" spans="1:65" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="30"/>
+      <c r="A26" s="33"/>
       <c r="B26" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="C26" s="10" t="s">
         <v>238</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="D26" s="10" t="s">
         <v>239</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="E26" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="F26" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="F26" s="10" t="s">
+      <c r="G26" s="10" t="s">
         <v>242</v>
       </c>
-      <c r="G26" s="10" t="s">
+      <c r="H26" s="10" t="s">
         <v>243</v>
       </c>
-      <c r="H26" s="10" t="s">
+      <c r="I26" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="I26" s="10" t="s">
+      <c r="J26" s="10" t="s">
         <v>245</v>
       </c>
-      <c r="J26" s="10" t="s">
+      <c r="K26" s="10" t="s">
         <v>246</v>
       </c>
-      <c r="K26" s="10" t="s">
+      <c r="L26" s="10" t="s">
         <v>247</v>
       </c>
-      <c r="L26" s="10" t="s">
+      <c r="M26" s="10" t="s">
         <v>248</v>
       </c>
-      <c r="M26" s="10" t="s">
+      <c r="N26" s="10" t="s">
         <v>249</v>
       </c>
-      <c r="N26" s="10" t="s">
+      <c r="O26" s="10" t="s">
+        <v>454</v>
+      </c>
+      <c r="P26" s="10" t="s">
+        <v>424</v>
+      </c>
+      <c r="Q26" s="10" t="s">
         <v>250</v>
       </c>
-      <c r="O26" s="10" t="s">
+      <c r="R26" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="S26" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="T26" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="U26" s="10" t="s">
         <v>455</v>
       </c>
-      <c r="P26" s="10" t="s">
+      <c r="V26" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="W26" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="X26" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="Y26" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="Z26" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="AA26" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="AB26" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="AC26" s="10" t="s">
+        <v>439</v>
+      </c>
+      <c r="AD26" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="AE26" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="AF26" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="AG26" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="AH26" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="AI26" s="10" t="s">
+        <v>266</v>
+      </c>
+      <c r="AJ26" s="10" t="s">
+        <v>267</v>
+      </c>
+      <c r="AK26" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="AL26" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="AM26" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="AN26" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="AO26" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="AP26" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="AQ26" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="AR26" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="AS26" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="AT26" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="AU26" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="AV26" s="10" t="s">
+        <v>279</v>
+      </c>
+      <c r="AW26" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="AX26" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="AY26" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="AZ26" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="BA26" s="10" t="s">
         <v>425</v>
       </c>
-      <c r="Q26" s="10" t="s">
-        <v>251</v>
-      </c>
-      <c r="R26" s="10" t="s">
-        <v>252</v>
-      </c>
-      <c r="S26" s="10" t="s">
-        <v>253</v>
-      </c>
-      <c r="T26" s="10" t="s">
-        <v>254</v>
-      </c>
-      <c r="U26" s="10" t="s">
-        <v>456</v>
-      </c>
-      <c r="V26" s="10" t="s">
-        <v>255</v>
-      </c>
-      <c r="W26" s="10" t="s">
-        <v>256</v>
-      </c>
-      <c r="X26" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="Y26" s="10" t="s">
-        <v>258</v>
-      </c>
-      <c r="Z26" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="AA26" s="10" t="s">
-        <v>260</v>
-      </c>
-      <c r="AB26" s="10" t="s">
-        <v>261</v>
-      </c>
-      <c r="AC26" s="10" t="s">
-        <v>440</v>
-      </c>
-      <c r="AD26" s="10" t="s">
-        <v>262</v>
-      </c>
-      <c r="AE26" s="10" t="s">
-        <v>263</v>
-      </c>
-      <c r="AF26" s="10" t="s">
-        <v>264</v>
-      </c>
-      <c r="AG26" s="10" t="s">
-        <v>265</v>
-      </c>
-      <c r="AH26" s="10" t="s">
-        <v>266</v>
-      </c>
-      <c r="AI26" s="10" t="s">
-        <v>267</v>
-      </c>
-      <c r="AJ26" s="10" t="s">
-        <v>268</v>
-      </c>
-      <c r="AK26" s="10" t="s">
-        <v>269</v>
-      </c>
-      <c r="AL26" s="10" t="s">
-        <v>270</v>
-      </c>
-      <c r="AM26" s="10" t="s">
-        <v>271</v>
-      </c>
-      <c r="AN26" s="10" t="s">
-        <v>272</v>
-      </c>
-      <c r="AO26" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="AP26" s="10" t="s">
-        <v>274</v>
-      </c>
-      <c r="AQ26" s="10" t="s">
-        <v>275</v>
-      </c>
-      <c r="AR26" s="10" t="s">
-        <v>276</v>
-      </c>
-      <c r="AS26" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="AT26" s="10" t="s">
-        <v>278</v>
-      </c>
-      <c r="AU26" s="10" t="s">
-        <v>279</v>
-      </c>
-      <c r="AV26" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="AW26" s="10" t="s">
-        <v>281</v>
-      </c>
-      <c r="AX26" s="10" t="s">
-        <v>282</v>
-      </c>
-      <c r="AY26" s="10" t="s">
-        <v>283</v>
-      </c>
-      <c r="AZ26" s="10" t="s">
+      <c r="BB26" s="10" t="s">
         <v>284</v>
       </c>
-      <c r="BA26" s="10" t="s">
-        <v>426</v>
-      </c>
-      <c r="BB26" s="10" t="s">
+      <c r="BC26" s="10" t="s">
         <v>285</v>
       </c>
-      <c r="BC26" s="10" t="s">
+      <c r="BD26" s="10" t="s">
         <v>286</v>
       </c>
-      <c r="BD26" s="10" t="s">
+      <c r="BE26" s="10" t="s">
         <v>287</v>
       </c>
-      <c r="BE26" s="10" t="s">
+      <c r="BF26" s="10" t="s">
         <v>288</v>
       </c>
-      <c r="BF26" s="10" t="s">
+      <c r="BG26" s="10" t="s">
         <v>289</v>
       </c>
-      <c r="BG26" s="10" t="s">
+      <c r="BH26" s="10" t="s">
         <v>290</v>
       </c>
-      <c r="BH26" s="10" t="s">
+      <c r="BI26" s="10" t="s">
         <v>291</v>
       </c>
-      <c r="BI26" s="10" t="s">
+      <c r="BJ26" s="10" t="s">
         <v>292</v>
       </c>
-      <c r="BJ26" s="10" t="s">
+      <c r="BK26" s="10" t="s">
         <v>293</v>
       </c>
-      <c r="BK26" s="10" t="s">
+      <c r="BL26" s="10" t="s">
         <v>294</v>
       </c>
-      <c r="BL26" s="10" t="s">
+      <c r="BM26" s="10" t="s">
         <v>295</v>
-      </c>
-      <c r="BM26" s="10" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="27" spans="1:65" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="30"/>
+      <c r="A27" s="33"/>
       <c r="B27" s="15" t="s">
+        <v>720</v>
+      </c>
+      <c r="C27" s="15" t="s">
         <v>721</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="D27" s="16" t="s">
         <v>722</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="E27" s="16" t="s">
         <v>723</v>
       </c>
-      <c r="E27" s="16" t="s">
+      <c r="F27" s="16" t="s">
         <v>724</v>
       </c>
-      <c r="F27" s="16" t="s">
+      <c r="G27" s="15" t="s">
         <v>725</v>
       </c>
-      <c r="G27" s="15" t="s">
+      <c r="H27" s="15" t="s">
         <v>726</v>
       </c>
-      <c r="H27" s="15" t="s">
+      <c r="I27" s="15" t="s">
         <v>727</v>
       </c>
-      <c r="I27" s="15" t="s">
+      <c r="J27" s="15" t="s">
         <v>728</v>
       </c>
-      <c r="J27" s="15" t="s">
+      <c r="K27" s="15" t="s">
         <v>729</v>
       </c>
-      <c r="K27" s="15" t="s">
+      <c r="L27" s="15" t="s">
         <v>730</v>
       </c>
-      <c r="L27" s="15" t="s">
+      <c r="M27" s="15" t="s">
         <v>731</v>
       </c>
-      <c r="M27" s="15" t="s">
+      <c r="N27" s="15" t="s">
         <v>732</v>
       </c>
-      <c r="N27" s="15" t="s">
+      <c r="O27" s="15" t="s">
         <v>733</v>
       </c>
-      <c r="O27" s="15" t="s">
+      <c r="P27" s="15" t="s">
         <v>734</v>
       </c>
-      <c r="P27" s="15" t="s">
+      <c r="Q27" s="15" t="s">
         <v>735</v>
       </c>
-      <c r="Q27" s="15" t="s">
+      <c r="R27" s="16" t="s">
         <v>736</v>
       </c>
-      <c r="R27" s="16" t="s">
+      <c r="S27" s="16" t="s">
         <v>737</v>
       </c>
-      <c r="S27" s="16" t="s">
+      <c r="T27" s="15" t="s">
         <v>738</v>
       </c>
-      <c r="T27" s="15" t="s">
+      <c r="U27" s="15" t="s">
         <v>739</v>
       </c>
-      <c r="U27" s="15" t="s">
+      <c r="V27" s="15" t="s">
         <v>740</v>
       </c>
-      <c r="V27" s="15" t="s">
+      <c r="W27" s="15" t="s">
         <v>741</v>
       </c>
-      <c r="W27" s="15" t="s">
+      <c r="X27" s="15" t="s">
         <v>742</v>
       </c>
-      <c r="X27" s="15" t="s">
+      <c r="Y27" s="15" t="s">
         <v>743</v>
       </c>
-      <c r="Y27" s="15" t="s">
+      <c r="Z27" s="15" t="s">
         <v>744</v>
       </c>
-      <c r="Z27" s="15" t="s">
+      <c r="AA27" s="15" t="s">
         <v>745</v>
       </c>
-      <c r="AA27" s="15" t="s">
+      <c r="AB27" s="15" t="s">
         <v>746</v>
       </c>
-      <c r="AB27" s="15" t="s">
+      <c r="AC27" s="15" t="s">
         <v>747</v>
       </c>
-      <c r="AC27" s="15" t="s">
+      <c r="AD27" s="15" t="s">
         <v>748</v>
       </c>
-      <c r="AD27" s="15" t="s">
+      <c r="AE27" s="15" t="s">
         <v>749</v>
       </c>
-      <c r="AE27" s="15" t="s">
+      <c r="AF27" s="15" t="s">
         <v>750</v>
       </c>
-      <c r="AF27" s="15" t="s">
+      <c r="AG27" s="15" t="s">
         <v>751</v>
       </c>
-      <c r="AG27" s="15" t="s">
+      <c r="AH27" s="16" t="s">
         <v>752</v>
       </c>
-      <c r="AH27" s="16" t="s">
+      <c r="AI27" s="16" t="s">
         <v>753</v>
       </c>
-      <c r="AI27" s="16" t="s">
+      <c r="AJ27" s="15" t="s">
         <v>754</v>
       </c>
-      <c r="AJ27" s="15" t="s">
+      <c r="AK27" s="15" t="s">
         <v>755</v>
       </c>
-      <c r="AK27" s="15" t="s">
+      <c r="AL27" s="15" t="s">
         <v>756</v>
       </c>
-      <c r="AL27" s="15" t="s">
+      <c r="AM27" s="15" t="s">
         <v>757</v>
       </c>
-      <c r="AM27" s="15" t="s">
+      <c r="AN27" s="15" t="s">
         <v>758</v>
       </c>
-      <c r="AN27" s="15" t="s">
+      <c r="AO27" s="15" t="s">
         <v>759</v>
       </c>
-      <c r="AO27" s="15" t="s">
+      <c r="AP27" s="15" t="s">
         <v>760</v>
       </c>
-      <c r="AP27" s="15" t="s">
+      <c r="AQ27" s="15" t="s">
         <v>761</v>
       </c>
-      <c r="AQ27" s="15" t="s">
+      <c r="AR27" s="15" t="s">
         <v>762</v>
       </c>
-      <c r="AR27" s="15" t="s">
+      <c r="AS27" s="15" t="s">
         <v>763</v>
       </c>
-      <c r="AS27" s="15" t="s">
+      <c r="AT27" s="15" t="s">
         <v>764</v>
       </c>
-      <c r="AT27" s="15" t="s">
+      <c r="AU27" s="15" t="s">
         <v>765</v>
       </c>
-      <c r="AU27" s="15" t="s">
+      <c r="AV27" s="15" t="s">
         <v>766</v>
       </c>
-      <c r="AV27" s="15" t="s">
+      <c r="AW27" s="15" t="s">
         <v>767</v>
       </c>
-      <c r="AW27" s="15" t="s">
+      <c r="AX27" s="16" t="s">
         <v>768</v>
       </c>
-      <c r="AX27" s="16" t="s">
+      <c r="AY27" s="15" t="s">
         <v>769</v>
       </c>
-      <c r="AY27" s="15" t="s">
+      <c r="AZ27" s="15" t="s">
         <v>770</v>
       </c>
-      <c r="AZ27" s="15" t="s">
+      <c r="BA27" s="15" t="s">
         <v>771</v>
       </c>
-      <c r="BA27" s="15" t="s">
+      <c r="BB27" s="15" t="s">
         <v>772</v>
       </c>
-      <c r="BB27" s="15" t="s">
+      <c r="BC27" s="15" t="s">
         <v>773</v>
       </c>
-      <c r="BC27" s="15" t="s">
+      <c r="BD27" s="15" t="s">
         <v>774</v>
       </c>
-      <c r="BD27" s="15" t="s">
+      <c r="BE27" s="15" t="s">
         <v>775</v>
       </c>
-      <c r="BE27" s="15" t="s">
+      <c r="BF27" s="15" t="s">
         <v>776</v>
       </c>
-      <c r="BF27" s="15" t="s">
+      <c r="BG27" s="15" t="s">
         <v>777</v>
       </c>
-      <c r="BG27" s="15" t="s">
+      <c r="BH27" s="15" t="s">
         <v>778</v>
       </c>
-      <c r="BH27" s="15" t="s">
+      <c r="BI27" s="15" t="s">
         <v>779</v>
       </c>
-      <c r="BI27" s="15" t="s">
+      <c r="BJ27" s="15" t="s">
         <v>780</v>
       </c>
-      <c r="BJ27" s="15" t="s">
+      <c r="BK27" s="15" t="s">
         <v>781</v>
       </c>
-      <c r="BK27" s="15" t="s">
+      <c r="BL27" s="15" t="s">
         <v>782</v>
       </c>
-      <c r="BL27" s="15" t="s">
+      <c r="BM27" s="15" t="s">
         <v>783</v>
-      </c>
-      <c r="BM27" s="15" t="s">
-        <v>784</v>
       </c>
     </row>
     <row r="28" spans="1:65" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="30" t="s">
-        <v>441</v>
+      <c r="A28" s="33" t="s">
+        <v>440</v>
       </c>
       <c r="B28" s="6">
         <v>281</v>
@@ -20561,393 +20581,393 @@
       </c>
     </row>
     <row r="29" spans="1:65" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="30"/>
+      <c r="A29" s="33"/>
       <c r="B29" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="C29" s="10" t="s">
         <v>297</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="D29" s="10" t="s">
         <v>298</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="E29" s="10" t="s">
         <v>299</v>
       </c>
-      <c r="E29" s="10" t="s">
+      <c r="F29" s="10" t="s">
         <v>300</v>
       </c>
-      <c r="F29" s="10" t="s">
+      <c r="G29" s="10" t="s">
         <v>301</v>
       </c>
-      <c r="G29" s="10" t="s">
+      <c r="H29" s="10" t="s">
+        <v>426</v>
+      </c>
+      <c r="I29" s="10" t="s">
         <v>302</v>
       </c>
-      <c r="H29" s="10" t="s">
+      <c r="J29" s="10" t="s">
         <v>427</v>
       </c>
-      <c r="I29" s="10" t="s">
+      <c r="K29" s="10" t="s">
         <v>303</v>
       </c>
-      <c r="J29" s="10" t="s">
+      <c r="L29" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="M29" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="N29" s="10" t="s">
+        <v>306</v>
+      </c>
+      <c r="O29" s="10" t="s">
+        <v>307</v>
+      </c>
+      <c r="P29" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="Q29" s="10" t="s">
+        <v>309</v>
+      </c>
+      <c r="R29" s="10" t="s">
+        <v>310</v>
+      </c>
+      <c r="S29" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="T29" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="U29" s="10" t="s">
+        <v>313</v>
+      </c>
+      <c r="V29" s="10" t="s">
+        <v>314</v>
+      </c>
+      <c r="W29" s="10" t="s">
+        <v>315</v>
+      </c>
+      <c r="X29" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="Y29" s="10" t="s">
+        <v>317</v>
+      </c>
+      <c r="Z29" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="AA29" s="10" t="s">
+        <v>319</v>
+      </c>
+      <c r="AB29" s="10" t="s">
+        <v>320</v>
+      </c>
+      <c r="AC29" s="10" t="s">
         <v>428</v>
       </c>
-      <c r="K29" s="10" t="s">
-        <v>304</v>
-      </c>
-      <c r="L29" s="10" t="s">
-        <v>305</v>
-      </c>
-      <c r="M29" s="10" t="s">
-        <v>306</v>
-      </c>
-      <c r="N29" s="10" t="s">
-        <v>307</v>
-      </c>
-      <c r="O29" s="10" t="s">
-        <v>308</v>
-      </c>
-      <c r="P29" s="10" t="s">
-        <v>309</v>
-      </c>
-      <c r="Q29" s="10" t="s">
-        <v>310</v>
-      </c>
-      <c r="R29" s="10" t="s">
-        <v>311</v>
-      </c>
-      <c r="S29" s="10" t="s">
-        <v>312</v>
-      </c>
-      <c r="T29" s="10" t="s">
-        <v>313</v>
-      </c>
-      <c r="U29" s="10" t="s">
-        <v>314</v>
-      </c>
-      <c r="V29" s="10" t="s">
-        <v>315</v>
-      </c>
-      <c r="W29" s="10" t="s">
-        <v>316</v>
-      </c>
-      <c r="X29" s="10" t="s">
-        <v>317</v>
-      </c>
-      <c r="Y29" s="10" t="s">
-        <v>318</v>
-      </c>
-      <c r="Z29" s="10" t="s">
-        <v>319</v>
-      </c>
-      <c r="AA29" s="10" t="s">
-        <v>320</v>
-      </c>
-      <c r="AB29" s="10" t="s">
+      <c r="AD29" s="10" t="s">
         <v>321</v>
       </c>
-      <c r="AC29" s="10" t="s">
+      <c r="AE29" s="10" t="s">
+        <v>322</v>
+      </c>
+      <c r="AF29" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="AG29" s="10" t="s">
+        <v>324</v>
+      </c>
+      <c r="AH29" s="10" t="s">
+        <v>325</v>
+      </c>
+      <c r="AI29" s="10" t="s">
+        <v>326</v>
+      </c>
+      <c r="AJ29" s="10" t="s">
+        <v>327</v>
+      </c>
+      <c r="AK29" s="10" t="s">
+        <v>328</v>
+      </c>
+      <c r="AL29" s="10" t="s">
+        <v>329</v>
+      </c>
+      <c r="AM29" s="10" t="s">
+        <v>330</v>
+      </c>
+      <c r="AN29" s="10" t="s">
         <v>429</v>
       </c>
-      <c r="AD29" s="10" t="s">
-        <v>322</v>
-      </c>
-      <c r="AE29" s="10" t="s">
-        <v>323</v>
-      </c>
-      <c r="AF29" s="10" t="s">
-        <v>324</v>
-      </c>
-      <c r="AG29" s="10" t="s">
-        <v>325</v>
-      </c>
-      <c r="AH29" s="10" t="s">
-        <v>326</v>
-      </c>
-      <c r="AI29" s="10" t="s">
-        <v>327</v>
-      </c>
-      <c r="AJ29" s="10" t="s">
-        <v>328</v>
-      </c>
-      <c r="AK29" s="10" t="s">
-        <v>329</v>
-      </c>
-      <c r="AL29" s="10" t="s">
-        <v>330</v>
-      </c>
-      <c r="AM29" s="10" t="s">
+      <c r="AO29" s="10" t="s">
         <v>331</v>
       </c>
-      <c r="AN29" s="10" t="s">
-        <v>430</v>
-      </c>
-      <c r="AO29" s="10" t="s">
+      <c r="AP29" s="10" t="s">
         <v>332</v>
       </c>
-      <c r="AP29" s="10" t="s">
+      <c r="AQ29" s="10" t="s">
         <v>333</v>
       </c>
-      <c r="AQ29" s="10" t="s">
+      <c r="AR29" s="10" t="s">
+        <v>441</v>
+      </c>
+      <c r="AS29" s="10" t="s">
         <v>334</v>
       </c>
-      <c r="AR29" s="10" t="s">
+      <c r="AT29" s="10" t="s">
+        <v>335</v>
+      </c>
+      <c r="AU29" s="10" t="s">
+        <v>336</v>
+      </c>
+      <c r="AV29" s="10" t="s">
+        <v>337</v>
+      </c>
+      <c r="AW29" s="10" t="s">
+        <v>338</v>
+      </c>
+      <c r="AX29" s="10" t="s">
+        <v>339</v>
+      </c>
+      <c r="AY29" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="AZ29" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="BA29" s="10" t="s">
+        <v>342</v>
+      </c>
+      <c r="BB29" s="10" t="s">
+        <v>343</v>
+      </c>
+      <c r="BC29" s="10" t="s">
+        <v>344</v>
+      </c>
+      <c r="BD29" s="10" t="s">
+        <v>345</v>
+      </c>
+      <c r="BE29" s="10" t="s">
+        <v>346</v>
+      </c>
+      <c r="BF29" s="10" t="s">
+        <v>347</v>
+      </c>
+      <c r="BG29" s="10" t="s">
+        <v>348</v>
+      </c>
+      <c r="BH29" s="10" t="s">
+        <v>349</v>
+      </c>
+      <c r="BI29" s="10" t="s">
+        <v>350</v>
+      </c>
+      <c r="BJ29" s="10" t="s">
+        <v>351</v>
+      </c>
+      <c r="BK29" s="10" t="s">
         <v>442</v>
       </c>
-      <c r="AS29" s="10" t="s">
-        <v>335</v>
-      </c>
-      <c r="AT29" s="10" t="s">
-        <v>336</v>
-      </c>
-      <c r="AU29" s="10" t="s">
-        <v>337</v>
-      </c>
-      <c r="AV29" s="10" t="s">
-        <v>338</v>
-      </c>
-      <c r="AW29" s="10" t="s">
-        <v>339</v>
-      </c>
-      <c r="AX29" s="10" t="s">
-        <v>340</v>
-      </c>
-      <c r="AY29" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="AZ29" s="10" t="s">
-        <v>342</v>
-      </c>
-      <c r="BA29" s="10" t="s">
-        <v>343</v>
-      </c>
-      <c r="BB29" s="10" t="s">
-        <v>344</v>
-      </c>
-      <c r="BC29" s="10" t="s">
-        <v>345</v>
-      </c>
-      <c r="BD29" s="10" t="s">
-        <v>346</v>
-      </c>
-      <c r="BE29" s="10" t="s">
-        <v>347</v>
-      </c>
-      <c r="BF29" s="10" t="s">
-        <v>348</v>
-      </c>
-      <c r="BG29" s="10" t="s">
-        <v>349</v>
-      </c>
-      <c r="BH29" s="10" t="s">
-        <v>350</v>
-      </c>
-      <c r="BI29" s="10" t="s">
-        <v>351</v>
-      </c>
-      <c r="BJ29" s="10" t="s">
+      <c r="BL29" s="10" t="s">
         <v>352</v>
       </c>
-      <c r="BK29" s="10" t="s">
-        <v>443</v>
-      </c>
-      <c r="BL29" s="10" t="s">
+      <c r="BM29" s="10" t="s">
         <v>353</v>
-      </c>
-      <c r="BM29" s="10" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="30" spans="1:65" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="30"/>
+      <c r="A30" s="33"/>
       <c r="B30" s="15" t="s">
+        <v>784</v>
+      </c>
+      <c r="C30" s="15" t="s">
         <v>785</v>
       </c>
-      <c r="C30" s="15" t="s">
+      <c r="D30" s="15" t="s">
         <v>786</v>
       </c>
-      <c r="D30" s="15" t="s">
+      <c r="E30" s="15" t="s">
         <v>787</v>
       </c>
-      <c r="E30" s="15" t="s">
+      <c r="F30" s="16" t="s">
         <v>788</v>
       </c>
-      <c r="F30" s="16" t="s">
+      <c r="G30" s="16" t="s">
         <v>789</v>
       </c>
-      <c r="G30" s="16" t="s">
+      <c r="H30" s="15" t="s">
         <v>790</v>
       </c>
-      <c r="H30" s="15" t="s">
+      <c r="I30" s="15" t="s">
         <v>791</v>
       </c>
-      <c r="I30" s="15" t="s">
+      <c r="J30" s="15" t="s">
         <v>792</v>
       </c>
-      <c r="J30" s="15" t="s">
+      <c r="K30" s="15" t="s">
         <v>793</v>
       </c>
-      <c r="K30" s="15" t="s">
+      <c r="L30" s="15" t="s">
         <v>794</v>
       </c>
-      <c r="L30" s="15" t="s">
+      <c r="M30" s="15" t="s">
         <v>795</v>
       </c>
-      <c r="M30" s="15" t="s">
+      <c r="N30" s="15" t="s">
         <v>796</v>
       </c>
-      <c r="N30" s="15" t="s">
+      <c r="O30" s="15" t="s">
         <v>797</v>
       </c>
-      <c r="O30" s="15" t="s">
+      <c r="P30" s="15" t="s">
         <v>798</v>
       </c>
-      <c r="P30" s="15" t="s">
+      <c r="Q30" s="15" t="s">
         <v>799</v>
       </c>
-      <c r="Q30" s="15" t="s">
+      <c r="R30" s="16" t="s">
         <v>800</v>
       </c>
-      <c r="R30" s="16" t="s">
+      <c r="S30" s="15" t="s">
         <v>801</v>
       </c>
-      <c r="S30" s="15" t="s">
+      <c r="T30" s="15" t="s">
         <v>802</v>
       </c>
-      <c r="T30" s="15" t="s">
+      <c r="U30" s="15" t="s">
         <v>803</v>
       </c>
-      <c r="U30" s="15" t="s">
+      <c r="V30" s="15" t="s">
         <v>804</v>
       </c>
-      <c r="V30" s="15" t="s">
+      <c r="W30" s="15" t="s">
         <v>805</v>
       </c>
-      <c r="W30" s="15" t="s">
+      <c r="X30" s="15" t="s">
         <v>806</v>
       </c>
-      <c r="X30" s="15" t="s">
+      <c r="Y30" s="15" t="s">
         <v>807</v>
       </c>
-      <c r="Y30" s="15" t="s">
+      <c r="Z30" s="15" t="s">
         <v>808</v>
       </c>
-      <c r="Z30" s="15" t="s">
+      <c r="AA30" s="15" t="s">
         <v>809</v>
       </c>
-      <c r="AA30" s="15" t="s">
+      <c r="AB30" s="15" t="s">
         <v>810</v>
       </c>
-      <c r="AB30" s="15" t="s">
+      <c r="AC30" s="15" t="s">
         <v>811</v>
       </c>
-      <c r="AC30" s="15" t="s">
+      <c r="AD30" s="15" t="s">
         <v>812</v>
       </c>
-      <c r="AD30" s="15" t="s">
+      <c r="AE30" s="15" t="s">
         <v>813</v>
       </c>
-      <c r="AE30" s="15" t="s">
+      <c r="AF30" s="15" t="s">
         <v>814</v>
       </c>
-      <c r="AF30" s="15" t="s">
+      <c r="AG30" s="15" t="s">
         <v>815</v>
       </c>
-      <c r="AG30" s="15" t="s">
+      <c r="AH30" s="16" t="s">
         <v>816</v>
       </c>
-      <c r="AH30" s="16" t="s">
+      <c r="AI30" s="16" t="s">
         <v>817</v>
       </c>
-      <c r="AI30" s="16" t="s">
+      <c r="AJ30" s="15" t="s">
         <v>818</v>
       </c>
-      <c r="AJ30" s="15" t="s">
+      <c r="AK30" s="15" t="s">
         <v>819</v>
       </c>
-      <c r="AK30" s="15" t="s">
+      <c r="AL30" s="15" t="s">
         <v>820</v>
       </c>
-      <c r="AL30" s="15" t="s">
+      <c r="AM30" s="15" t="s">
         <v>821</v>
       </c>
-      <c r="AM30" s="15" t="s">
+      <c r="AN30" s="15" t="s">
         <v>822</v>
       </c>
-      <c r="AN30" s="15" t="s">
+      <c r="AO30" s="15" t="s">
         <v>823</v>
       </c>
-      <c r="AO30" s="15" t="s">
+      <c r="AP30" s="15" t="s">
         <v>824</v>
       </c>
-      <c r="AP30" s="15" t="s">
+      <c r="AQ30" s="15" t="s">
         <v>825</v>
       </c>
-      <c r="AQ30" s="15" t="s">
+      <c r="AR30" s="15" t="s">
         <v>826</v>
       </c>
-      <c r="AR30" s="15" t="s">
+      <c r="AS30" s="15" t="s">
         <v>827</v>
       </c>
-      <c r="AS30" s="15" t="s">
+      <c r="AT30" s="15" t="s">
         <v>828</v>
       </c>
-      <c r="AT30" s="15" t="s">
+      <c r="AU30" s="15" t="s">
         <v>829</v>
       </c>
-      <c r="AU30" s="15" t="s">
+      <c r="AV30" s="15" t="s">
         <v>830</v>
       </c>
-      <c r="AV30" s="15" t="s">
+      <c r="AW30" s="15" t="s">
         <v>831</v>
       </c>
-      <c r="AW30" s="15" t="s">
+      <c r="AX30" s="16" t="s">
         <v>832</v>
       </c>
-      <c r="AX30" s="16" t="s">
+      <c r="AY30" s="15" t="s">
         <v>833</v>
       </c>
-      <c r="AY30" s="15" t="s">
+      <c r="AZ30" s="15" t="s">
         <v>834</v>
       </c>
-      <c r="AZ30" s="15" t="s">
+      <c r="BA30" s="15" t="s">
         <v>835</v>
       </c>
-      <c r="BA30" s="15" t="s">
+      <c r="BB30" s="15" t="s">
         <v>836</v>
       </c>
-      <c r="BB30" s="15" t="s">
+      <c r="BC30" s="15" t="s">
         <v>837</v>
       </c>
-      <c r="BC30" s="15" t="s">
+      <c r="BD30" s="15" t="s">
         <v>838</v>
       </c>
-      <c r="BD30" s="15" t="s">
+      <c r="BE30" s="15" t="s">
         <v>839</v>
       </c>
-      <c r="BE30" s="15" t="s">
+      <c r="BF30" s="15" t="s">
         <v>840</v>
       </c>
-      <c r="BF30" s="15" t="s">
+      <c r="BG30" s="15" t="s">
         <v>841</v>
       </c>
-      <c r="BG30" s="15" t="s">
+      <c r="BH30" s="15" t="s">
         <v>842</v>
       </c>
-      <c r="BH30" s="15" t="s">
+      <c r="BI30" s="15" t="s">
         <v>843</v>
       </c>
-      <c r="BI30" s="15" t="s">
+      <c r="BJ30" s="15" t="s">
         <v>844</v>
       </c>
-      <c r="BJ30" s="15" t="s">
+      <c r="BK30" s="15" t="s">
         <v>845</v>
       </c>
-      <c r="BK30" s="15" t="s">
+      <c r="BL30" s="15" t="s">
         <v>846</v>
       </c>
-      <c r="BL30" s="15" t="s">
+      <c r="BM30" s="15" t="s">
         <v>847</v>
-      </c>
-      <c r="BM30" s="15" t="s">
-        <v>848</v>
       </c>
     </row>
     <row r="31" spans="1:65" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -21019,6 +21039,164 @@
     </row>
   </sheetData>
   <mergeCells count="182">
+    <mergeCell ref="BK21:BK23"/>
+    <mergeCell ref="BL21:BL23"/>
+    <mergeCell ref="BM21:BM23"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="D21:D23"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="BJ21:BJ23"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="BJ18:BJ20"/>
+    <mergeCell ref="BK18:BK20"/>
+    <mergeCell ref="BL18:BL20"/>
+    <mergeCell ref="BM18:BM20"/>
+    <mergeCell ref="BL12:BL14"/>
+    <mergeCell ref="BM12:BM14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="BJ15:BJ17"/>
+    <mergeCell ref="BK15:BK17"/>
+    <mergeCell ref="BL15:BL17"/>
+    <mergeCell ref="BM15:BM17"/>
+    <mergeCell ref="BK9:BK11"/>
+    <mergeCell ref="BL9:BL11"/>
+    <mergeCell ref="BM9:BM11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="BJ12:BJ14"/>
+    <mergeCell ref="BK12:BK14"/>
+    <mergeCell ref="AO9:AO11"/>
+    <mergeCell ref="AP9:AP11"/>
+    <mergeCell ref="AQ9:AQ11"/>
+    <mergeCell ref="AR9:AR11"/>
+    <mergeCell ref="AS9:AS11"/>
+    <mergeCell ref="BJ9:BJ11"/>
+    <mergeCell ref="AI9:AI11"/>
+    <mergeCell ref="AJ9:AJ11"/>
+    <mergeCell ref="AK9:AK11"/>
+    <mergeCell ref="AL9:AL11"/>
+    <mergeCell ref="AM9:AM11"/>
+    <mergeCell ref="AN9:AN11"/>
+    <mergeCell ref="AC9:AC11"/>
+    <mergeCell ref="AD9:AD11"/>
+    <mergeCell ref="AE9:AE11"/>
+    <mergeCell ref="AF9:AF11"/>
+    <mergeCell ref="AG9:AG11"/>
+    <mergeCell ref="AH9:AH11"/>
+    <mergeCell ref="W9:W11"/>
+    <mergeCell ref="X9:X11"/>
+    <mergeCell ref="Y9:Y11"/>
+    <mergeCell ref="Z9:Z11"/>
+    <mergeCell ref="AA9:AA11"/>
+    <mergeCell ref="AB9:AB11"/>
+    <mergeCell ref="Q9:Q11"/>
+    <mergeCell ref="R9:R11"/>
+    <mergeCell ref="S9:S11"/>
+    <mergeCell ref="T9:T11"/>
+    <mergeCell ref="U9:U11"/>
+    <mergeCell ref="V9:V11"/>
+    <mergeCell ref="K9:K11"/>
+    <mergeCell ref="L9:L11"/>
+    <mergeCell ref="M9:M11"/>
+    <mergeCell ref="N9:N11"/>
+    <mergeCell ref="O9:O11"/>
+    <mergeCell ref="P9:P11"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="J9:J11"/>
+    <mergeCell ref="AR6:AR8"/>
+    <mergeCell ref="AS6:AS8"/>
+    <mergeCell ref="BJ6:BJ8"/>
+    <mergeCell ref="AF6:AF8"/>
+    <mergeCell ref="AG6:AG8"/>
+    <mergeCell ref="AH6:AH8"/>
+    <mergeCell ref="AI6:AI8"/>
+    <mergeCell ref="AJ6:AJ8"/>
+    <mergeCell ref="AK6:AK8"/>
+    <mergeCell ref="Z6:Z8"/>
+    <mergeCell ref="AA6:AA8"/>
+    <mergeCell ref="AB6:AB8"/>
+    <mergeCell ref="AC6:AC8"/>
+    <mergeCell ref="AD6:AD8"/>
+    <mergeCell ref="AE6:AE8"/>
+    <mergeCell ref="T6:T8"/>
+    <mergeCell ref="U6:U8"/>
+    <mergeCell ref="V6:V8"/>
+    <mergeCell ref="N6:N8"/>
+    <mergeCell ref="O6:O8"/>
+    <mergeCell ref="P6:P8"/>
+    <mergeCell ref="Q6:Q8"/>
+    <mergeCell ref="R6:R8"/>
+    <mergeCell ref="S6:S8"/>
+    <mergeCell ref="BK6:BK8"/>
+    <mergeCell ref="BL6:BL8"/>
+    <mergeCell ref="BM6:BM8"/>
+    <mergeCell ref="AL6:AL8"/>
+    <mergeCell ref="AM6:AM8"/>
+    <mergeCell ref="AN6:AN8"/>
+    <mergeCell ref="AO6:AO8"/>
+    <mergeCell ref="AP6:AP8"/>
+    <mergeCell ref="AQ6:AQ8"/>
+    <mergeCell ref="BA3:BA5"/>
+    <mergeCell ref="BB3:BB5"/>
+    <mergeCell ref="BC3:BC5"/>
+    <mergeCell ref="BD3:BD5"/>
+    <mergeCell ref="AS3:AS5"/>
+    <mergeCell ref="AT3:AT5"/>
+    <mergeCell ref="W6:W8"/>
+    <mergeCell ref="X6:X8"/>
+    <mergeCell ref="Y6:Y8"/>
+    <mergeCell ref="AU3:AU5"/>
+    <mergeCell ref="AV3:AV5"/>
+    <mergeCell ref="AW3:AW5"/>
+    <mergeCell ref="AX3:AX5"/>
+    <mergeCell ref="AM3:AM5"/>
+    <mergeCell ref="AR3:AR5"/>
+    <mergeCell ref="AD3:AD5"/>
+    <mergeCell ref="AE3:AE5"/>
+    <mergeCell ref="AF3:AF5"/>
+    <mergeCell ref="BM3:BM5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="J6:J8"/>
+    <mergeCell ref="K6:K8"/>
+    <mergeCell ref="L6:L8"/>
+    <mergeCell ref="M6:M8"/>
+    <mergeCell ref="BE3:BE5"/>
+    <mergeCell ref="BF3:BF5"/>
+    <mergeCell ref="BG3:BG5"/>
+    <mergeCell ref="BJ3:BJ5"/>
+    <mergeCell ref="BK3:BK5"/>
+    <mergeCell ref="BL3:BL5"/>
+    <mergeCell ref="AY3:AY5"/>
+    <mergeCell ref="AZ3:AZ5"/>
+    <mergeCell ref="S3:S5"/>
+    <mergeCell ref="T3:T5"/>
+    <mergeCell ref="AG3:AG5"/>
+    <mergeCell ref="AA3:AA5"/>
+    <mergeCell ref="AB3:AB5"/>
+    <mergeCell ref="AC3:AC5"/>
     <mergeCell ref="AA1:AP1"/>
     <mergeCell ref="AI3:AJ5"/>
     <mergeCell ref="I3:I5"/>
@@ -21043,164 +21221,6 @@
     <mergeCell ref="P3:P5"/>
     <mergeCell ref="Q3:Q5"/>
     <mergeCell ref="R3:R5"/>
-    <mergeCell ref="BM3:BM5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="E6:E8"/>
-    <mergeCell ref="J6:J8"/>
-    <mergeCell ref="K6:K8"/>
-    <mergeCell ref="L6:L8"/>
-    <mergeCell ref="M6:M8"/>
-    <mergeCell ref="BE3:BE5"/>
-    <mergeCell ref="BF3:BF5"/>
-    <mergeCell ref="BG3:BG5"/>
-    <mergeCell ref="BJ3:BJ5"/>
-    <mergeCell ref="BK3:BK5"/>
-    <mergeCell ref="BL3:BL5"/>
-    <mergeCell ref="AY3:AY5"/>
-    <mergeCell ref="AZ3:AZ5"/>
-    <mergeCell ref="S3:S5"/>
-    <mergeCell ref="T3:T5"/>
-    <mergeCell ref="AG3:AG5"/>
-    <mergeCell ref="AA3:AA5"/>
-    <mergeCell ref="AB3:AB5"/>
-    <mergeCell ref="AC3:AC5"/>
-    <mergeCell ref="BA3:BA5"/>
-    <mergeCell ref="BB3:BB5"/>
-    <mergeCell ref="BC3:BC5"/>
-    <mergeCell ref="BD3:BD5"/>
-    <mergeCell ref="AS3:AS5"/>
-    <mergeCell ref="AT3:AT5"/>
-    <mergeCell ref="W6:W8"/>
-    <mergeCell ref="X6:X8"/>
-    <mergeCell ref="Y6:Y8"/>
-    <mergeCell ref="AU3:AU5"/>
-    <mergeCell ref="AV3:AV5"/>
-    <mergeCell ref="AW3:AW5"/>
-    <mergeCell ref="AX3:AX5"/>
-    <mergeCell ref="AM3:AM5"/>
-    <mergeCell ref="AR3:AR5"/>
-    <mergeCell ref="AD3:AD5"/>
-    <mergeCell ref="AE3:AE5"/>
-    <mergeCell ref="AF3:AF5"/>
-    <mergeCell ref="N6:N8"/>
-    <mergeCell ref="O6:O8"/>
-    <mergeCell ref="P6:P8"/>
-    <mergeCell ref="Q6:Q8"/>
-    <mergeCell ref="R6:R8"/>
-    <mergeCell ref="S6:S8"/>
-    <mergeCell ref="BK6:BK8"/>
-    <mergeCell ref="BL6:BL8"/>
-    <mergeCell ref="BM6:BM8"/>
-    <mergeCell ref="AL6:AL8"/>
-    <mergeCell ref="AM6:AM8"/>
-    <mergeCell ref="AN6:AN8"/>
-    <mergeCell ref="AO6:AO8"/>
-    <mergeCell ref="AP6:AP8"/>
-    <mergeCell ref="AQ6:AQ8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="J9:J11"/>
-    <mergeCell ref="AR6:AR8"/>
-    <mergeCell ref="AS6:AS8"/>
-    <mergeCell ref="BJ6:BJ8"/>
-    <mergeCell ref="AF6:AF8"/>
-    <mergeCell ref="AG6:AG8"/>
-    <mergeCell ref="AH6:AH8"/>
-    <mergeCell ref="AI6:AI8"/>
-    <mergeCell ref="AJ6:AJ8"/>
-    <mergeCell ref="AK6:AK8"/>
-    <mergeCell ref="Z6:Z8"/>
-    <mergeCell ref="AA6:AA8"/>
-    <mergeCell ref="AB6:AB8"/>
-    <mergeCell ref="AC6:AC8"/>
-    <mergeCell ref="AD6:AD8"/>
-    <mergeCell ref="AE6:AE8"/>
-    <mergeCell ref="T6:T8"/>
-    <mergeCell ref="U6:U8"/>
-    <mergeCell ref="V6:V8"/>
-    <mergeCell ref="Q9:Q11"/>
-    <mergeCell ref="R9:R11"/>
-    <mergeCell ref="S9:S11"/>
-    <mergeCell ref="T9:T11"/>
-    <mergeCell ref="U9:U11"/>
-    <mergeCell ref="V9:V11"/>
-    <mergeCell ref="K9:K11"/>
-    <mergeCell ref="L9:L11"/>
-    <mergeCell ref="M9:M11"/>
-    <mergeCell ref="N9:N11"/>
-    <mergeCell ref="O9:O11"/>
-    <mergeCell ref="P9:P11"/>
-    <mergeCell ref="AE9:AE11"/>
-    <mergeCell ref="AF9:AF11"/>
-    <mergeCell ref="AG9:AG11"/>
-    <mergeCell ref="AH9:AH11"/>
-    <mergeCell ref="W9:W11"/>
-    <mergeCell ref="X9:X11"/>
-    <mergeCell ref="Y9:Y11"/>
-    <mergeCell ref="Z9:Z11"/>
-    <mergeCell ref="AA9:AA11"/>
-    <mergeCell ref="AB9:AB11"/>
-    <mergeCell ref="BK9:BK11"/>
-    <mergeCell ref="BL9:BL11"/>
-    <mergeCell ref="BM9:BM11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="E12:E14"/>
-    <mergeCell ref="BJ12:BJ14"/>
-    <mergeCell ref="BK12:BK14"/>
-    <mergeCell ref="AO9:AO11"/>
-    <mergeCell ref="AP9:AP11"/>
-    <mergeCell ref="AQ9:AQ11"/>
-    <mergeCell ref="AR9:AR11"/>
-    <mergeCell ref="AS9:AS11"/>
-    <mergeCell ref="BJ9:BJ11"/>
-    <mergeCell ref="AI9:AI11"/>
-    <mergeCell ref="AJ9:AJ11"/>
-    <mergeCell ref="AK9:AK11"/>
-    <mergeCell ref="AL9:AL11"/>
-    <mergeCell ref="AM9:AM11"/>
-    <mergeCell ref="AN9:AN11"/>
-    <mergeCell ref="AC9:AC11"/>
-    <mergeCell ref="AD9:AD11"/>
-    <mergeCell ref="BL12:BL14"/>
-    <mergeCell ref="BM12:BM14"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="BJ15:BJ17"/>
-    <mergeCell ref="BK15:BK17"/>
-    <mergeCell ref="BL15:BL17"/>
-    <mergeCell ref="BM15:BM17"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="BJ18:BJ20"/>
-    <mergeCell ref="BK18:BK20"/>
-    <mergeCell ref="BL18:BL20"/>
-    <mergeCell ref="BM18:BM20"/>
-    <mergeCell ref="BK21:BK23"/>
-    <mergeCell ref="BL21:BL23"/>
-    <mergeCell ref="BM21:BM23"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="D21:D23"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="BJ21:BJ23"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0" right="7.8740157480314977E-3" top="1.9685039370078741" bottom="0" header="0.31496062992125984" footer="0"/>

</xml_diff>